<commit_message>
Calculating and interpreting liquidity ratios
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FE55AA-05E4-B34B-A2E0-459BC2CA4ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66DE0B7-4BA0-1746-87F4-D11821A6044B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="950" activeTab="3" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="950" activeTab="3" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -2039,41 +2039,47 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2081,23 +2087,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2473,7 +2473,7 @@
   <dimension ref="B3:I49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="274" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="264" t="s">
+      <c r="F5" s="274" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="265"/>
+      <c r="D6" s="275"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3264,19 +3264,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="264" t="s">
+      <c r="D14" s="274" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="264" t="s">
+      <c r="F14" s="274" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="264" t="s">
+      <c r="H14" s="274" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3289,15 +3289,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="265"/>
+      <c r="D15" s="275"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="265"/>
+      <c r="F15" s="275"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="265"/>
+      <c r="H15" s="275"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3475,16 +3475,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="J23:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4669,7 +4669,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4679,7 +4679,7 @@
         <f>'P&amp;L'!D11</f>
         <v>191504</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.5300408933626928</v>
@@ -4688,17 +4688,17 @@
         <f>'P&amp;L'!E11</f>
         <v>172829</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4706,15 +4706,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4725,7 +4725,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4735,7 +4735,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>48.472512323502379</v>
@@ -4744,17 +4744,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>53.570812768690445</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="264" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4762,15 +4762,15 @@
         <f>G5</f>
         <v>7.5300408933626928</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4781,7 +4781,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4791,7 +4791,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4800,17 +4800,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4818,15 +4818,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4837,7 +4837,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4847,7 +4847,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4856,17 +4856,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4874,15 +4874,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4893,7 +4893,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4903,7 +4903,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4912,12 +4912,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -4925,7 +4925,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -4933,15 +4933,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -4952,7 +4952,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -4962,7 +4962,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -4971,17 +4971,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="274" t="s">
+      <c r="M25" s="266" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -4989,15 +4989,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="275"/>
+      <c r="M26" s="267"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5008,34 +5008,34 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="268" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="42"/>
-      <c r="F29" s="264"/>
+      <c r="F29" s="274"/>
       <c r="G29" s="44"/>
       <c r="I29" s="42"/>
-      <c r="J29" s="264"/>
+      <c r="J29" s="274"/>
       <c r="K29" s="44"/>
-      <c r="M29" s="268" t="s">
+      <c r="M29" s="264" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="269"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="45"/>
-      <c r="F30" s="265"/>
+      <c r="F30" s="275"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="265"/>
+      <c r="J30" s="275"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="265"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5046,34 +5046,34 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="266" t="s">
+      <c r="B33" s="268" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="42"/>
-      <c r="F33" s="264"/>
+      <c r="F33" s="274"/>
       <c r="G33" s="44"/>
       <c r="I33" s="42"/>
-      <c r="J33" s="264"/>
+      <c r="J33" s="274"/>
       <c r="K33" s="44"/>
-      <c r="M33" s="268" t="s">
+      <c r="M33" s="264" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="267"/>
+      <c r="B34" s="269"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="45"/>
-      <c r="F34" s="265"/>
+      <c r="F34" s="275"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45"/>
-      <c r="J34" s="265"/>
+      <c r="J34" s="275"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="265"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5090,34 +5090,34 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="266" t="s">
+      <c r="B37" s="268" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="42"/>
-      <c r="F37" s="264"/>
+      <c r="F37" s="274"/>
       <c r="G37" s="44"/>
       <c r="I37" s="42"/>
-      <c r="J37" s="264"/>
+      <c r="J37" s="274"/>
       <c r="K37" s="44"/>
-      <c r="M37" s="268" t="s">
+      <c r="M37" s="264" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="267"/>
+      <c r="B38" s="269"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="45"/>
-      <c r="F38" s="265"/>
+      <c r="F38" s="275"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45"/>
-      <c r="J38" s="265"/>
+      <c r="J38" s="275"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="269"/>
+      <c r="M38" s="265"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5153,7 +5153,7 @@
         <f>I41+I43-I45</f>
         <v>68.548621585483062</v>
       </c>
-      <c r="M41" s="268" t="s">
+      <c r="M41" s="264" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5217,51 +5217,65 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="269"/>
+      <c r="M45" s="265"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="266" t="s">
+      <c r="B48" s="268" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="42"/>
-      <c r="F48" s="264"/>
+      <c r="F48" s="274"/>
       <c r="G48" s="44"/>
       <c r="I48" s="42"/>
-      <c r="J48" s="264"/>
+      <c r="J48" s="274"/>
       <c r="K48" s="44"/>
-      <c r="M48" s="268" t="s">
+      <c r="M48" s="264" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="267"/>
+      <c r="B49" s="269"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="45"/>
-      <c r="F49" s="265"/>
+      <c r="F49" s="275"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45"/>
-      <c r="J49" s="265"/>
+      <c r="J49" s="275"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="269"/>
+      <c r="M49" s="265"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="M37:M38"/>
@@ -5278,27 +5292,13 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="M41:M45"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5312,7 +5312,9 @@
   </sheetPr>
   <dimension ref="B3:M18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5322,7 +5324,7 @@
     <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="8.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
@@ -5355,135 +5357,216 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="53"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="53"/>
-      <c r="M5" s="274" t="s">
+      <c r="E5" s="42">
+        <f>BS!D22</f>
+        <v>70907</v>
+      </c>
+      <c r="F5" s="274"/>
+      <c r="G5" s="53">
+        <f>E5/E6</f>
+        <v>2.250872960446956</v>
+      </c>
+      <c r="I5" s="42">
+        <f>BS!E22</f>
+        <v>61001</v>
+      </c>
+      <c r="J5" s="274"/>
+      <c r="K5" s="53">
+        <f>I5/I6</f>
+        <v>1.8897459727385377</v>
+      </c>
+      <c r="M5" s="266" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="265"/>
+      <c r="E6" s="45">
+        <f>BS!D45</f>
+        <v>31502</v>
+      </c>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="265"/>
+      <c r="I6" s="45">
+        <f>BS!E45</f>
+        <v>32280</v>
+      </c>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="275"/>
+      <c r="M6" s="267"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="264"/>
-      <c r="G9" s="53"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="264"/>
-      <c r="K9" s="53"/>
-      <c r="M9" s="274" t="s">
+      <c r="E9" s="59">
+        <f>SUM(BS!D19:D21)</f>
+        <v>45538</v>
+      </c>
+      <c r="F9" s="274"/>
+      <c r="G9" s="53">
+        <f>E9/E10</f>
+        <v>1.4455590121262143</v>
+      </c>
+      <c r="I9" s="42">
+        <f>SUM(BS!E19:E21)</f>
+        <v>37243</v>
+      </c>
+      <c r="J9" s="274"/>
+      <c r="K9" s="53">
+        <f>I9/I10</f>
+        <v>1.1537484510532838</v>
+      </c>
+      <c r="M9" s="266" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="265"/>
+      <c r="E10" s="65">
+        <f>BS!D45</f>
+        <v>31502</v>
+      </c>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="265"/>
+      <c r="I10" s="45">
+        <f>BS!E45</f>
+        <v>32280</v>
+      </c>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="275"/>
+      <c r="M10" s="267"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="264"/>
-      <c r="G13" s="53"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="264"/>
-      <c r="K13" s="53"/>
-      <c r="M13" s="274" t="s">
+      <c r="E13" s="59">
+        <f>SUM((BS!D20:D21))</f>
+        <v>19291</v>
+      </c>
+      <c r="F13" s="274"/>
+      <c r="G13" s="53">
+        <f>E13/E14</f>
+        <v>0.61237381753539455</v>
+      </c>
+      <c r="I13" s="42">
+        <f>SUM(BS!E20:E21)</f>
+        <v>12626</v>
+      </c>
+      <c r="J13" s="274"/>
+      <c r="K13" s="53">
+        <f>I13/I14</f>
+        <v>0.39114002478314747</v>
+      </c>
+      <c r="M13" s="266" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="265"/>
+      <c r="E14" s="65">
+        <f>BS!D45</f>
+        <v>31502</v>
+      </c>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="265"/>
+      <c r="I14" s="45">
+        <f>BS!E45</f>
+        <v>32280</v>
+      </c>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="275"/>
+      <c r="M14" s="267"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="264"/>
-      <c r="G17" s="53"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="264"/>
-      <c r="K17" s="53"/>
-      <c r="M17" s="274" t="s">
+      <c r="E17" s="59">
+        <f>SUM(BS!D19:D21)</f>
+        <v>45538</v>
+      </c>
+      <c r="F17" s="274"/>
+      <c r="G17" s="53">
+        <f>E17/E18</f>
+        <v>94.282108296368563</v>
+      </c>
+      <c r="I17" s="42">
+        <f>SUM(BS!E19:E21)</f>
+        <v>37243</v>
+      </c>
+      <c r="J17" s="274"/>
+      <c r="K17" s="53">
+        <f>I17/I18</f>
+        <v>84.148560144604573</v>
+      </c>
+      <c r="M17" s="266" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="265"/>
+      <c r="E18" s="65">
+        <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
+        <v>482.99726027397259</v>
+      </c>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="265"/>
+      <c r="I18" s="45">
+        <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
+        <v>442.58630136986301</v>
+      </c>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="275"/>
+      <c r="M18" s="267"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5494,15 +5577,6 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5559,7 +5633,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5567,28 +5641,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="66"/>
       <c r="I5" s="42"/>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="66"/>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="45"/>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45"/>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5607,7 +5681,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5615,28 +5689,28 @@
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="59"/>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="66"/>
       <c r="I9" s="59"/>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="66"/>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="264" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="65"/>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65"/>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5645,7 +5719,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5653,28 +5727,28 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="59"/>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="66"/>
       <c r="I13" s="59"/>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="66"/>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="65"/>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65"/>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5683,7 +5757,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5691,28 +5765,28 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="59"/>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="71"/>
       <c r="I17" s="59"/>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="71"/>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="65"/>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65"/>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -5721,7 +5795,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5729,34 +5803,34 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="71"/>
       <c r="I21" s="59"/>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="71"/>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="65"/>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65"/>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -5764,38 +5838,41 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="71"/>
       <c r="I25" s="59"/>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="71"/>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="264" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="65"/>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65"/>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -5806,16 +5883,13 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5879,7 +5953,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5887,28 +5961,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="72"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="72"/>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="65"/>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5925,7 +5999,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5933,28 +6007,28 @@
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="42"/>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="72"/>
       <c r="I9" s="42"/>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="72"/>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="264" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45"/>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -5971,7 +6045,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5979,31 +6053,31 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="59"/>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="72"/>
       <c r="I13" s="59"/>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="72"/>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="45"/>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45"/>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6011,31 +6085,31 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="42"/>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="72"/>
       <c r="I17" s="42"/>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="72"/>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="45"/>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6043,28 +6117,28 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="72"/>
       <c r="I21" s="59"/>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="72"/>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="45"/>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6079,7 +6153,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6087,31 +6161,31 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="72"/>
       <c r="I25" s="59"/>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="72"/>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="264" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="45"/>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="268" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6119,31 +6193,31 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="264"/>
+      <c r="F29" s="274"/>
       <c r="G29" s="72"/>
       <c r="I29" s="59"/>
-      <c r="J29" s="264"/>
+      <c r="J29" s="274"/>
       <c r="K29" s="72"/>
-      <c r="M29" s="268" t="s">
+      <c r="M29" s="264" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="269"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="265"/>
+      <c r="F30" s="275"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="265"/>
+      <c r="J30" s="275"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="265"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="278" t="s">
+      <c r="B33" s="276" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6151,59 +6225,36 @@
       </c>
       <c r="D33" s="73"/>
       <c r="E33" s="246"/>
-      <c r="F33" s="276"/>
+      <c r="F33" s="278"/>
       <c r="G33" s="247"/>
       <c r="H33" s="73"/>
       <c r="I33" s="246"/>
-      <c r="J33" s="276"/>
+      <c r="J33" s="278"/>
       <c r="K33" s="247"/>
-      <c r="M33" s="268" t="s">
+      <c r="M33" s="264" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="279"/>
+      <c r="B34" s="277"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="249"/>
-      <c r="F34" s="277"/>
+      <c r="F34" s="279"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249"/>
-      <c r="J34" s="277"/>
+      <c r="J34" s="279"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="265"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6216,6 +6267,29 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6280,7 +6354,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6288,28 +6362,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="71"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="113"/>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="65"/>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6330,38 +6404,38 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>186</v>
       </c>
       <c r="E9" s="116"/>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="71"/>
       <c r="I9" s="196"/>
-      <c r="J9" s="276"/>
+      <c r="J9" s="278"/>
       <c r="K9" s="197"/>
       <c r="L9" s="73"/>
-      <c r="M9" s="282" t="s">
+      <c r="M9" s="280" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
       <c r="E10" s="117"/>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198"/>
-      <c r="J10" s="277"/>
+      <c r="J10" s="279"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="283"/>
+      <c r="M10" s="281"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6375,131 +6449,131 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>190</v>
       </c>
       <c r="E13" s="119"/>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="71"/>
       <c r="I13" s="119"/>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="113"/>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="120"/>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120"/>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>198</v>
       </c>
       <c r="E17" s="116"/>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="250"/>
       <c r="I17" s="116"/>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="250"/>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
       <c r="E18" s="117"/>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117"/>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>199</v>
       </c>
       <c r="E21" s="42"/>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="66"/>
       <c r="I21" s="42"/>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="66"/>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E22" s="45"/>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>204</v>
       </c>
       <c r="E25" s="42"/>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="66"/>
       <c r="I25" s="42"/>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="66"/>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="264" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E26" s="45"/>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="280" t="s">
+      <c r="B29" s="282" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="281"/>
+      <c r="C29" s="283"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
@@ -6513,12 +6587,15 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -6532,15 +6609,12 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculating and interpreting solvency ratios
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66DE0B7-4BA0-1746-87F4-D11821A6044B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FDBD9E-E423-8D4C-88AA-CDCF51B78D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="950" activeTab="3" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="950" activeTab="4" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -2039,40 +2039,46 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2081,23 +2087,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2473,7 +2473,7 @@
   <dimension ref="B3:I49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="274" t="s">
+      <c r="D5" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="274" t="s">
+      <c r="F5" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="275"/>
+      <c r="D6" s="265"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3264,19 +3264,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="274" t="s">
+      <c r="D14" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="274" t="s">
+      <c r="F14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="274" t="s">
+      <c r="H14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3289,15 +3289,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="275"/>
+      <c r="D15" s="265"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="275"/>
+      <c r="F15" s="265"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="275"/>
+      <c r="H15" s="265"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3475,16 +3475,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4669,7 +4669,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4679,7 +4679,7 @@
         <f>'P&amp;L'!D11</f>
         <v>191504</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.5300408933626928</v>
@@ -4688,17 +4688,17 @@
         <f>'P&amp;L'!E11</f>
         <v>172829</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4706,15 +4706,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4725,7 +4725,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4735,7 +4735,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>48.472512323502379</v>
@@ -4744,17 +4744,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>53.570812768690445</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4762,15 +4762,15 @@
         <f>G5</f>
         <v>7.5300408933626928</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4781,7 +4781,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4791,7 +4791,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4800,17 +4800,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4818,15 +4818,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4837,7 +4837,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4847,7 +4847,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4856,17 +4856,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4874,15 +4874,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4893,7 +4893,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4903,7 +4903,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4912,12 +4912,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -4925,7 +4925,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -4933,15 +4933,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -4952,7 +4952,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -4962,7 +4962,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -4971,17 +4971,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="266" t="s">
+      <c r="M25" s="274" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -4989,15 +4989,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="267"/>
+      <c r="M26" s="275"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5008,34 +5008,34 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="42"/>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="44"/>
       <c r="I29" s="42"/>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="44"/>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="45"/>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5046,34 +5046,34 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="268" t="s">
+      <c r="B33" s="266" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="42"/>
-      <c r="F33" s="274"/>
+      <c r="F33" s="264"/>
       <c r="G33" s="44"/>
       <c r="I33" s="42"/>
-      <c r="J33" s="274"/>
+      <c r="J33" s="264"/>
       <c r="K33" s="44"/>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="269"/>
+      <c r="B34" s="267"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="45"/>
-      <c r="F34" s="275"/>
+      <c r="F34" s="265"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45"/>
-      <c r="J34" s="275"/>
+      <c r="J34" s="265"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5090,34 +5090,34 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="268" t="s">
+      <c r="B37" s="266" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="42"/>
-      <c r="F37" s="274"/>
+      <c r="F37" s="264"/>
       <c r="G37" s="44"/>
       <c r="I37" s="42"/>
-      <c r="J37" s="274"/>
+      <c r="J37" s="264"/>
       <c r="K37" s="44"/>
-      <c r="M37" s="264" t="s">
+      <c r="M37" s="268" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="269"/>
+      <c r="B38" s="267"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="45"/>
-      <c r="F38" s="275"/>
+      <c r="F38" s="265"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45"/>
-      <c r="J38" s="275"/>
+      <c r="J38" s="265"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="265"/>
+      <c r="M38" s="269"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5153,7 +5153,7 @@
         <f>I41+I43-I45</f>
         <v>68.548621585483062</v>
       </c>
-      <c r="M41" s="264" t="s">
+      <c r="M41" s="268" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5217,44 +5217,72 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="265"/>
+      <c r="M45" s="269"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="268" t="s">
+      <c r="B48" s="266" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="42"/>
-      <c r="F48" s="274"/>
+      <c r="F48" s="264"/>
       <c r="G48" s="44"/>
       <c r="I48" s="42"/>
-      <c r="J48" s="274"/>
+      <c r="J48" s="264"/>
       <c r="K48" s="44"/>
-      <c r="M48" s="264" t="s">
+      <c r="M48" s="268" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="269"/>
+      <c r="B49" s="267"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="45"/>
-      <c r="F49" s="275"/>
+      <c r="F49" s="265"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45"/>
-      <c r="J49" s="275"/>
+      <c r="J49" s="265"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="265"/>
+      <c r="M49" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F37:F38"/>
@@ -5271,34 +5299,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5312,7 +5312,7 @@
   </sheetPr>
   <dimension ref="B3:M18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5357,7 +5357,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5368,7 +5368,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5377,17 +5377,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="266" t="s">
+      <c r="M5" s="274" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5396,18 +5396,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="267"/>
+      <c r="M6" s="275"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5418,7 +5418,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5427,17 +5427,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="266" t="s">
+      <c r="M9" s="274" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5446,18 +5446,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="267"/>
+      <c r="M10" s="275"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5468,7 +5468,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5477,17 +5477,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="266" t="s">
+      <c r="M13" s="274" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5496,18 +5496,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="267"/>
+      <c r="M14" s="275"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5518,7 +5518,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5527,17 +5527,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="266" t="s">
+      <c r="M17" s="274" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5546,27 +5546,18 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="267"/>
+      <c r="M18" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5577,6 +5568,15 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5590,7 +5590,9 @@
   </sheetPr>
   <dimension ref="B3:M26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5633,36 +5635,54 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="274"/>
-      <c r="G5" s="66"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="274"/>
-      <c r="K5" s="66"/>
-      <c r="M5" s="264" t="s">
+      <c r="E5" s="42">
+        <f>BS!D42+BS!D36</f>
+        <v>29474</v>
+      </c>
+      <c r="F5" s="264"/>
+      <c r="G5" s="66">
+        <f>E5/E6</f>
+        <v>0.2242426086824206</v>
+      </c>
+      <c r="I5" s="42">
+        <f>BS!E42+BS!E36</f>
+        <v>35016</v>
+      </c>
+      <c r="J5" s="264"/>
+      <c r="K5" s="66">
+        <f>I5/I6</f>
+        <v>0.30774639222372607</v>
+      </c>
+      <c r="M5" s="268" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="275"/>
+      <c r="E6" s="45">
+        <f>BS!D32</f>
+        <v>131438</v>
+      </c>
+      <c r="F6" s="265"/>
       <c r="G6" s="67"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="275"/>
+      <c r="I6" s="45">
+        <f>BS!E32</f>
+        <v>113782</v>
+      </c>
+      <c r="J6" s="265"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5681,36 +5701,54 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>69</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="274"/>
-      <c r="G9" s="66"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="274"/>
-      <c r="K9" s="66"/>
-      <c r="M9" s="264" t="s">
+      <c r="E9" s="59">
+        <f>E5</f>
+        <v>29474</v>
+      </c>
+      <c r="F9" s="264"/>
+      <c r="G9" s="66">
+        <f>E9/E10</f>
+        <v>0.18316843989261211</v>
+      </c>
+      <c r="I9" s="59">
+        <f>I5</f>
+        <v>35016</v>
+      </c>
+      <c r="J9" s="264"/>
+      <c r="K9" s="66">
+        <f>I9/I10</f>
+        <v>0.23532574362558636</v>
+      </c>
+      <c r="M9" s="268" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="275"/>
+      <c r="E10" s="65">
+        <f>BS!D32+BS!D36+BS!D42</f>
+        <v>160912</v>
+      </c>
+      <c r="F10" s="265"/>
       <c r="G10" s="67"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="275"/>
+      <c r="I10" s="65">
+        <f>I6+I5</f>
+        <v>148798</v>
+      </c>
+      <c r="J10" s="265"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5719,36 +5757,54 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="274"/>
-      <c r="G13" s="66"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="274"/>
-      <c r="K13" s="66"/>
-      <c r="M13" s="264" t="s">
+      <c r="E13" s="59">
+        <f>E9</f>
+        <v>29474</v>
+      </c>
+      <c r="F13" s="264"/>
+      <c r="G13" s="66">
+        <f>E13/E14</f>
+        <v>0.16262324749918616</v>
+      </c>
+      <c r="I13" s="59">
+        <f>I9</f>
+        <v>35016</v>
+      </c>
+      <c r="J13" s="264"/>
+      <c r="K13" s="66">
+        <f>I13/I14</f>
+        <v>0.20809413442681404</v>
+      </c>
+      <c r="M13" s="268" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="275"/>
+      <c r="E14" s="65">
+        <f>BS!D23</f>
+        <v>181241</v>
+      </c>
+      <c r="F14" s="265"/>
       <c r="G14" s="67"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="275"/>
+      <c r="I14" s="65">
+        <f>BS!E23</f>
+        <v>168270</v>
+      </c>
+      <c r="J14" s="265"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5757,36 +5813,54 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>75</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="274"/>
-      <c r="G17" s="71"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="274"/>
-      <c r="K17" s="71"/>
-      <c r="M17" s="264" t="s">
+      <c r="E17" s="59">
+        <f>'P&amp;L'!D24</f>
+        <v>22551.000000000004</v>
+      </c>
+      <c r="F17" s="264"/>
+      <c r="G17" s="71">
+        <f>E17/E18</f>
+        <v>8.2755963302752313</v>
+      </c>
+      <c r="I17" s="59">
+        <f>'P&amp;L'!E24</f>
+        <v>18597.000000000004</v>
+      </c>
+      <c r="J17" s="264"/>
+      <c r="K17" s="71">
+        <f>I17/I18</f>
+        <v>6.2155748663101615</v>
+      </c>
+      <c r="M17" s="268" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="275"/>
+      <c r="E18" s="65">
+        <f>'P&amp;L'!D26 * -1</f>
+        <v>2725</v>
+      </c>
+      <c r="F18" s="265"/>
       <c r="G18" s="67"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="275"/>
+      <c r="I18" s="65">
+        <f>'P&amp;L'!E26*-1</f>
+        <v>2992</v>
+      </c>
+      <c r="J18" s="265"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -5795,84 +5869,117 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="274"/>
-      <c r="G21" s="71"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="274"/>
-      <c r="K21" s="71"/>
-      <c r="M21" s="264" t="s">
+      <c r="E21" s="59">
+        <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
+        <v>24832.000000000004</v>
+      </c>
+      <c r="F21" s="264"/>
+      <c r="G21" s="71">
+        <f>E21/E22</f>
+        <v>4.9604474630443471</v>
+      </c>
+      <c r="I21" s="59">
+        <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
+        <v>21072.000000000004</v>
+      </c>
+      <c r="J21" s="264"/>
+      <c r="K21" s="71">
+        <f>I21/I22</f>
+        <v>3.8543991220047564</v>
+      </c>
+      <c r="M21" s="268" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="275"/>
+      <c r="E22" s="65">
+        <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
+        <v>5006</v>
+      </c>
+      <c r="F22" s="265"/>
       <c r="G22" s="67"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="275"/>
+      <c r="I22" s="65">
+        <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
+        <v>5467</v>
+      </c>
+      <c r="J22" s="265"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="21"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="274"/>
-      <c r="G25" s="71"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="274"/>
-      <c r="K25" s="71"/>
-      <c r="M25" s="264" t="s">
+      <c r="E25" s="59">
+        <f>AVERAGE(BS!D23:E23)</f>
+        <v>174755.5</v>
+      </c>
+      <c r="F25" s="264"/>
+      <c r="G25" s="71">
+        <f>E25/E26</f>
+        <v>1.4252956528831253</v>
+      </c>
+      <c r="I25" s="59">
+        <f>AVERAGE(BS!E23:F23)</f>
+        <v>164911.5</v>
+      </c>
+      <c r="J25" s="264"/>
+      <c r="K25" s="71">
+        <f>I25/I26</f>
+        <v>1.5516336179521557</v>
+      </c>
+      <c r="M25" s="268" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="21"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="275"/>
+      <c r="E26" s="65">
+        <f>AVERAGE(BS!D32:E32)</f>
+        <v>122610</v>
+      </c>
+      <c r="F26" s="265"/>
       <c r="G26" s="67"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="275"/>
+      <c r="I26" s="65">
+        <f>AVERAGE(BS!E32:F32)</f>
+        <v>106282.5</v>
+      </c>
+      <c r="J26" s="265"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -5883,13 +5990,16 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5953,7 +6063,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5961,28 +6071,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="72"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="72"/>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="65"/>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5999,7 +6109,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6007,28 +6117,28 @@
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="42"/>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="72"/>
       <c r="I9" s="42"/>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="72"/>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45"/>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6045,7 +6155,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6053,31 +6163,31 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="59"/>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="72"/>
       <c r="I13" s="59"/>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="72"/>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="45"/>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45"/>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6085,31 +6195,31 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="42"/>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="72"/>
       <c r="I17" s="42"/>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="72"/>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="45"/>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6117,28 +6227,28 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="59"/>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="72"/>
       <c r="I21" s="59"/>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="72"/>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="45"/>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6153,7 +6263,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6161,31 +6271,31 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="72"/>
       <c r="I25" s="59"/>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="72"/>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="45"/>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6193,31 +6303,31 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="72"/>
       <c r="I29" s="59"/>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="72"/>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="276" t="s">
+      <c r="B33" s="278" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6225,36 +6335,59 @@
       </c>
       <c r="D33" s="73"/>
       <c r="E33" s="246"/>
-      <c r="F33" s="278"/>
+      <c r="F33" s="276"/>
       <c r="G33" s="247"/>
       <c r="H33" s="73"/>
       <c r="I33" s="246"/>
-      <c r="J33" s="278"/>
+      <c r="J33" s="276"/>
       <c r="K33" s="247"/>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="277"/>
+      <c r="B34" s="279"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="249"/>
-      <c r="F34" s="279"/>
+      <c r="F34" s="277"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249"/>
-      <c r="J34" s="279"/>
+      <c r="J34" s="277"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6267,29 +6400,6 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6354,7 +6464,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6362,28 +6472,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="71"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="113"/>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="65"/>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6404,38 +6514,38 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>186</v>
       </c>
       <c r="E9" s="116"/>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="71"/>
       <c r="I9" s="196"/>
-      <c r="J9" s="278"/>
+      <c r="J9" s="276"/>
       <c r="K9" s="197"/>
       <c r="L9" s="73"/>
-      <c r="M9" s="280" t="s">
+      <c r="M9" s="282" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
       <c r="E10" s="117"/>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198"/>
-      <c r="J10" s="279"/>
+      <c r="J10" s="277"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="281"/>
+      <c r="M10" s="283"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6449,131 +6559,131 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>190</v>
       </c>
       <c r="E13" s="119"/>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="71"/>
       <c r="I13" s="119"/>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="113"/>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="120"/>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120"/>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>198</v>
       </c>
       <c r="E17" s="116"/>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="250"/>
       <c r="I17" s="116"/>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="250"/>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
       <c r="E18" s="117"/>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117"/>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>199</v>
       </c>
       <c r="E21" s="42"/>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="66"/>
       <c r="I21" s="42"/>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="66"/>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E22" s="45"/>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>204</v>
       </c>
       <c r="E25" s="42"/>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="66"/>
       <c r="I25" s="42"/>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="66"/>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E26" s="45"/>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="282" t="s">
+      <c r="B29" s="280" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="283"/>
+      <c r="C29" s="281"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
@@ -6587,15 +6697,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -6609,12 +6716,15 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculating and interpreting profitability ratios
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FDBD9E-E423-8D4C-88AA-CDCF51B78D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF913AEC-599A-D548-8197-BF29CA93E3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="950" activeTab="4" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="950" activeTab="5" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -2039,41 +2039,47 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2081,23 +2087,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2473,11 +2473,11 @@
   <dimension ref="B3:I49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="274" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="264" t="s">
+      <c r="F5" s="274" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="265"/>
+      <c r="D6" s="275"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3264,19 +3264,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="264" t="s">
+      <c r="D14" s="274" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="264" t="s">
+      <c r="F14" s="274" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="264" t="s">
+      <c r="H14" s="274" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3289,15 +3289,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="265"/>
+      <c r="D15" s="275"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="265"/>
+      <c r="F15" s="275"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="265"/>
+      <c r="H15" s="275"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3475,16 +3475,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="J23:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4669,7 +4669,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4679,7 +4679,7 @@
         <f>'P&amp;L'!D11</f>
         <v>191504</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.5300408933626928</v>
@@ -4688,17 +4688,17 @@
         <f>'P&amp;L'!E11</f>
         <v>172829</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4706,15 +4706,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4725,7 +4725,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4735,7 +4735,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>48.472512323502379</v>
@@ -4744,17 +4744,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>53.570812768690445</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="264" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4762,15 +4762,15 @@
         <f>G5</f>
         <v>7.5300408933626928</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4781,7 +4781,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4791,7 +4791,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4800,17 +4800,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4818,15 +4818,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4837,7 +4837,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4847,7 +4847,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4856,17 +4856,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4874,15 +4874,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4893,7 +4893,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4903,7 +4903,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4912,12 +4912,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -4925,7 +4925,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -4933,15 +4933,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -4952,7 +4952,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -4962,7 +4962,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -4971,17 +4971,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="274" t="s">
+      <c r="M25" s="266" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -4989,15 +4989,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="275"/>
+      <c r="M26" s="267"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5008,34 +5008,34 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="268" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="42"/>
-      <c r="F29" s="264"/>
+      <c r="F29" s="274"/>
       <c r="G29" s="44"/>
       <c r="I29" s="42"/>
-      <c r="J29" s="264"/>
+      <c r="J29" s="274"/>
       <c r="K29" s="44"/>
-      <c r="M29" s="268" t="s">
+      <c r="M29" s="264" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="269"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="45"/>
-      <c r="F30" s="265"/>
+      <c r="F30" s="275"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="265"/>
+      <c r="J30" s="275"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="265"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5046,34 +5046,34 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="266" t="s">
+      <c r="B33" s="268" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="42"/>
-      <c r="F33" s="264"/>
+      <c r="F33" s="274"/>
       <c r="G33" s="44"/>
       <c r="I33" s="42"/>
-      <c r="J33" s="264"/>
+      <c r="J33" s="274"/>
       <c r="K33" s="44"/>
-      <c r="M33" s="268" t="s">
+      <c r="M33" s="264" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="267"/>
+      <c r="B34" s="269"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="45"/>
-      <c r="F34" s="265"/>
+      <c r="F34" s="275"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45"/>
-      <c r="J34" s="265"/>
+      <c r="J34" s="275"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="265"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5090,34 +5090,34 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="266" t="s">
+      <c r="B37" s="268" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="42"/>
-      <c r="F37" s="264"/>
+      <c r="F37" s="274"/>
       <c r="G37" s="44"/>
       <c r="I37" s="42"/>
-      <c r="J37" s="264"/>
+      <c r="J37" s="274"/>
       <c r="K37" s="44"/>
-      <c r="M37" s="268" t="s">
+      <c r="M37" s="264" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="267"/>
+      <c r="B38" s="269"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="45"/>
-      <c r="F38" s="265"/>
+      <c r="F38" s="275"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45"/>
-      <c r="J38" s="265"/>
+      <c r="J38" s="275"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="269"/>
+      <c r="M38" s="265"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5153,7 +5153,7 @@
         <f>I41+I43-I45</f>
         <v>68.548621585483062</v>
       </c>
-      <c r="M41" s="268" t="s">
+      <c r="M41" s="264" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5217,51 +5217,65 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="269"/>
+      <c r="M45" s="265"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="266" t="s">
+      <c r="B48" s="268" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="42"/>
-      <c r="F48" s="264"/>
+      <c r="F48" s="274"/>
       <c r="G48" s="44"/>
       <c r="I48" s="42"/>
-      <c r="J48" s="264"/>
+      <c r="J48" s="274"/>
       <c r="K48" s="44"/>
-      <c r="M48" s="268" t="s">
+      <c r="M48" s="264" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="267"/>
+      <c r="B49" s="269"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="45"/>
-      <c r="F49" s="265"/>
+      <c r="F49" s="275"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45"/>
-      <c r="J49" s="265"/>
+      <c r="J49" s="275"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="269"/>
+      <c r="M49" s="265"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="M37:M38"/>
@@ -5278,27 +5292,13 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="M41:M45"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5357,7 +5357,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5368,7 +5368,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5377,17 +5377,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="274" t="s">
+      <c r="M5" s="266" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5396,18 +5396,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="275"/>
+      <c r="M6" s="267"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5418,7 +5418,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5427,17 +5427,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="274" t="s">
+      <c r="M9" s="266" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5446,18 +5446,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="275"/>
+      <c r="M10" s="267"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5468,7 +5468,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5477,17 +5477,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="274" t="s">
+      <c r="M13" s="266" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5496,18 +5496,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="275"/>
+      <c r="M14" s="267"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5518,7 +5518,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5527,17 +5527,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="274" t="s">
+      <c r="M17" s="266" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5546,18 +5546,27 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="275"/>
+      <c r="M18" s="267"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5568,15 +5577,6 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5590,7 +5590,7 @@
   </sheetPr>
   <dimension ref="B3:M26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -5635,7 +5635,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5646,7 +5646,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="66">
         <f>E5/E6</f>
         <v>0.2242426086824206</v>
@@ -5655,17 +5655,17 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
@@ -5674,15 +5674,15 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5701,7 +5701,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5712,7 +5712,7 @@
         <f>E5</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="66">
         <f>E9/E10</f>
         <v>0.18316843989261211</v>
@@ -5721,17 +5721,17 @@
         <f>I5</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="274"/>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="264" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
@@ -5740,15 +5740,15 @@
         <f>BS!D32+BS!D36+BS!D42</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>I6+I5</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="275"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5757,7 +5757,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5768,7 +5768,7 @@
         <f>E9</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="66">
         <f>E13/E14</f>
         <v>0.16262324749918616</v>
@@ -5777,17 +5777,17 @@
         <f>I9</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
@@ -5796,15 +5796,15 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5813,7 +5813,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5824,7 +5824,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="71">
         <f>E17/E18</f>
         <v>8.2755963302752313</v>
@@ -5833,17 +5833,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
@@ -5852,15 +5852,15 @@
         <f>'P&amp;L'!D26 * -1</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>'P&amp;L'!E26*-1</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -5869,7 +5869,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5880,7 +5880,7 @@
         <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="71">
         <f>E21/E22</f>
         <v>4.9604474630443471</v>
@@ -5889,17 +5889,17 @@
         <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
@@ -5908,21 +5908,21 @@
         <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -5933,7 +5933,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="71">
         <f>E25/E26</f>
         <v>1.4252956528831253</v>
@@ -5942,17 +5942,17 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="264" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
@@ -5961,25 +5961,28 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -5990,16 +5993,13 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6013,7 +6013,9 @@
   </sheetPr>
   <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6063,36 +6065,54 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="72"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="72"/>
-      <c r="M5" s="268" t="s">
+      <c r="E5" s="59">
+        <f>'P&amp;L'!D17</f>
+        <v>48553.16</v>
+      </c>
+      <c r="F5" s="274"/>
+      <c r="G5" s="72">
+        <f>E5/E6</f>
+        <v>0.24417591591440571</v>
+      </c>
+      <c r="I5" s="59">
+        <f>'P&amp;L'!E17</f>
+        <v>41525.160000000003</v>
+      </c>
+      <c r="J5" s="274"/>
+      <c r="K5" s="72">
+        <f>I5/I6</f>
+        <v>0.23051476343530902</v>
+      </c>
+      <c r="M5" s="264" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="265"/>
+      <c r="E6" s="65">
+        <f>'P&amp;L'!D13</f>
+        <v>198845</v>
+      </c>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="265"/>
+      <c r="I6" s="65">
+        <f>'P&amp;L'!E13</f>
+        <v>180141</v>
+      </c>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -6109,36 +6129,54 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>151</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="264"/>
-      <c r="G9" s="72"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="264"/>
-      <c r="K9" s="72"/>
-      <c r="M9" s="268" t="s">
+      <c r="E9" s="42">
+        <f>'P&amp;L'!D24</f>
+        <v>22551.000000000004</v>
+      </c>
+      <c r="F9" s="274"/>
+      <c r="G9" s="72">
+        <f>E9/E10</f>
+        <v>0.11340994241746086</v>
+      </c>
+      <c r="I9" s="42">
+        <f>'P&amp;L'!E24</f>
+        <v>18597.000000000004</v>
+      </c>
+      <c r="J9" s="274"/>
+      <c r="K9" s="72">
+        <f>I9/I10</f>
+        <v>0.1032357986244109</v>
+      </c>
+      <c r="M9" s="264" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="265"/>
+      <c r="E10" s="45">
+        <f>E6</f>
+        <v>198845</v>
+      </c>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="265"/>
+      <c r="I10" s="45">
+        <f>I6</f>
+        <v>180141</v>
+      </c>
+      <c r="J10" s="275"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="265"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6155,100 +6193,154 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="264"/>
-      <c r="G13" s="72"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="264"/>
-      <c r="K13" s="72"/>
-      <c r="M13" s="268" t="s">
+      <c r="E13" s="59">
+        <f>'P&amp;L'!D28</f>
+        <v>19826.000000000004</v>
+      </c>
+      <c r="F13" s="274"/>
+      <c r="G13" s="72">
+        <f>E13/E14</f>
+        <v>9.9705801000779526E-2</v>
+      </c>
+      <c r="I13" s="59">
+        <f>'P&amp;L'!E28</f>
+        <v>15605.000000000004</v>
+      </c>
+      <c r="J13" s="274"/>
+      <c r="K13" s="72">
+        <f>I13/I14</f>
+        <v>8.6626586951332588E-2</v>
+      </c>
+      <c r="M13" s="264" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="265"/>
+      <c r="E14" s="45">
+        <f>E10</f>
+        <v>198845</v>
+      </c>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="265"/>
+      <c r="I14" s="45">
+        <f>I10</f>
+        <v>180141</v>
+      </c>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>80</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="264"/>
-      <c r="G17" s="72"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="264"/>
-      <c r="K17" s="72"/>
-      <c r="M17" s="268" t="s">
+      <c r="E17" s="42">
+        <f>'P&amp;L'!D32</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F17" s="274"/>
+      <c r="G17" s="72">
+        <f>E17/E18</f>
+        <v>8.9003998088963782E-2</v>
+      </c>
+      <c r="I17" s="42">
+        <f>'P&amp;L'!E32</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J17" s="274"/>
+      <c r="K17" s="72">
+        <f>I17/I18</f>
+        <v>7.7505953669625482E-2</v>
+      </c>
+      <c r="M17" s="264" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="265"/>
+      <c r="E18" s="45">
+        <f>E14</f>
+        <v>198845</v>
+      </c>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="265"/>
+      <c r="I18" s="45">
+        <f>I14</f>
+        <v>180141</v>
+      </c>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="264"/>
-      <c r="G21" s="72"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="264"/>
-      <c r="K21" s="72"/>
-      <c r="M21" s="268" t="s">
+      <c r="E21" s="59">
+        <f>E17</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F21" s="274"/>
+      <c r="G21" s="72">
+        <f>E21/E22</f>
+        <v>0.10127292131005892</v>
+      </c>
+      <c r="I21" s="59">
+        <f>I17</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J21" s="274"/>
+      <c r="K21" s="72">
+        <f>I21/I22</f>
+        <v>8.4663592290410331E-2</v>
+      </c>
+      <c r="M21" s="264" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="265"/>
+      <c r="E22" s="45">
+        <f>AVERAGE(BS!D23:E23)</f>
+        <v>174755.5</v>
+      </c>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="265"/>
+      <c r="I22" s="45">
+        <f>AVERAGE(BS!E23:F23)</f>
+        <v>164911.5</v>
+      </c>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6263,131 +6355,162 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>177</v>
       </c>
       <c r="D25" s="21"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="264"/>
-      <c r="G25" s="72"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="264"/>
-      <c r="K25" s="72"/>
-      <c r="M25" s="268" t="s">
+      <c r="E25" s="59">
+        <f>E9</f>
+        <v>22551.000000000004</v>
+      </c>
+      <c r="F25" s="274"/>
+      <c r="G25" s="72">
+        <f>E25/E26</f>
+        <v>0.1290431488565453</v>
+      </c>
+      <c r="I25" s="59">
+        <f>I9</f>
+        <v>18597.000000000004</v>
+      </c>
+      <c r="J25" s="274"/>
+      <c r="K25" s="72">
+        <f>I25/I26</f>
+        <v>0.11276957640916493</v>
+      </c>
+      <c r="M25" s="264" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="21"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="265"/>
+      <c r="E26" s="45">
+        <f>E22</f>
+        <v>174755.5</v>
+      </c>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="265"/>
+      <c r="I26" s="45">
+        <f>I22</f>
+        <v>164911.5</v>
+      </c>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="268" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>177</v>
       </c>
       <c r="D29" s="21"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="264"/>
-      <c r="G29" s="72"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="264"/>
-      <c r="K29" s="72"/>
-      <c r="M29" s="268" t="s">
+      <c r="E29" s="59">
+        <f>E9</f>
+        <v>22551.000000000004</v>
+      </c>
+      <c r="F29" s="274"/>
+      <c r="G29" s="72">
+        <f>E29/E30</f>
+        <v>0.14562655387297796</v>
+      </c>
+      <c r="I29" s="59">
+        <f>I9</f>
+        <v>18597.000000000004</v>
+      </c>
+      <c r="J29" s="274"/>
+      <c r="K29" s="72">
+        <f>I29/I30</f>
+        <v>0.1276687765161397</v>
+      </c>
+      <c r="M29" s="264" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="269"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
       <c r="D30" s="21"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="265"/>
+      <c r="E30" s="45">
+        <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
+        <v>154855</v>
+      </c>
+      <c r="F30" s="275"/>
       <c r="G30" s="46"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="265"/>
+      <c r="I30" s="45">
+        <f>AVERAGE(BS!E32:F32) + AVERAGE(BS!E36:F36) + AVERAGE(BS!E42:F42)</f>
+        <v>145666</v>
+      </c>
+      <c r="J30" s="275"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="265"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="278" t="s">
+      <c r="B33" s="276" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
         <v>80</v>
       </c>
       <c r="D33" s="73"/>
-      <c r="E33" s="246"/>
-      <c r="F33" s="276"/>
-      <c r="G33" s="247"/>
+      <c r="E33" s="246">
+        <f>E17</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F33" s="278"/>
+      <c r="G33" s="247">
+        <f>E33/E34</f>
+        <v>0.14434385449800183</v>
+      </c>
       <c r="H33" s="73"/>
-      <c r="I33" s="246"/>
-      <c r="J33" s="276"/>
-      <c r="K33" s="247"/>
-      <c r="M33" s="268" t="s">
+      <c r="I33" s="246">
+        <f>I17</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J33" s="278"/>
+      <c r="K33" s="247">
+        <f>I33/I34</f>
+        <v>0.13136687601439562</v>
+      </c>
+      <c r="M33" s="264" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="279"/>
+      <c r="B34" s="277"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="73"/>
-      <c r="E34" s="249"/>
-      <c r="F34" s="277"/>
+      <c r="E34" s="249">
+        <f>AVERAGE(BS!D32:E32)</f>
+        <v>122610</v>
+      </c>
+      <c r="F34" s="279"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
-      <c r="I34" s="249"/>
-      <c r="J34" s="277"/>
+      <c r="I34" s="249">
+        <f>AVERAGE(BS!E32:F32)</f>
+        <v>106282.5</v>
+      </c>
+      <c r="J34" s="279"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="265"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6400,6 +6523,29 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6464,7 +6610,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="268" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6472,28 +6618,28 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="59"/>
-      <c r="F5" s="264"/>
+      <c r="F5" s="274"/>
       <c r="G5" s="71"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="264"/>
+      <c r="J5" s="274"/>
       <c r="K5" s="113"/>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="264" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="269"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="65"/>
-      <c r="F6" s="265"/>
+      <c r="F6" s="275"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="265"/>
+      <c r="J6" s="275"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="265"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6514,38 +6660,38 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="268" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>186</v>
       </c>
       <c r="E9" s="116"/>
-      <c r="F9" s="264"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="71"/>
       <c r="I9" s="196"/>
-      <c r="J9" s="276"/>
+      <c r="J9" s="278"/>
       <c r="K9" s="197"/>
       <c r="L9" s="73"/>
-      <c r="M9" s="282" t="s">
+      <c r="M9" s="280" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="269"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
       <c r="E10" s="117"/>
-      <c r="F10" s="265"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198"/>
-      <c r="J10" s="277"/>
+      <c r="J10" s="279"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="283"/>
+      <c r="M10" s="281"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6559,131 +6705,131 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="268" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>190</v>
       </c>
       <c r="E13" s="119"/>
-      <c r="F13" s="264"/>
+      <c r="F13" s="274"/>
       <c r="G13" s="71"/>
       <c r="I13" s="119"/>
-      <c r="J13" s="264"/>
+      <c r="J13" s="274"/>
       <c r="K13" s="113"/>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="264" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="269"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="120"/>
-      <c r="F14" s="265"/>
+      <c r="F14" s="275"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120"/>
-      <c r="J14" s="265"/>
+      <c r="J14" s="275"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="265"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="268" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>198</v>
       </c>
       <c r="E17" s="116"/>
-      <c r="F17" s="264"/>
+      <c r="F17" s="274"/>
       <c r="G17" s="250"/>
       <c r="I17" s="116"/>
-      <c r="J17" s="264"/>
+      <c r="J17" s="274"/>
       <c r="K17" s="250"/>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="264" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="269"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
       <c r="E18" s="117"/>
-      <c r="F18" s="265"/>
+      <c r="F18" s="275"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117"/>
-      <c r="J18" s="265"/>
+      <c r="J18" s="275"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="265"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="268" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>199</v>
       </c>
       <c r="E21" s="42"/>
-      <c r="F21" s="264"/>
+      <c r="F21" s="274"/>
       <c r="G21" s="66"/>
       <c r="I21" s="42"/>
-      <c r="J21" s="264"/>
+      <c r="J21" s="274"/>
       <c r="K21" s="66"/>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="264" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="269"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E22" s="45"/>
-      <c r="F22" s="265"/>
+      <c r="F22" s="275"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="265"/>
+      <c r="J22" s="275"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="265"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="268" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>204</v>
       </c>
       <c r="E25" s="42"/>
-      <c r="F25" s="264"/>
+      <c r="F25" s="274"/>
       <c r="G25" s="66"/>
       <c r="I25" s="42"/>
-      <c r="J25" s="264"/>
+      <c r="J25" s="274"/>
       <c r="K25" s="66"/>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="264" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="269"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E26" s="45"/>
-      <c r="F26" s="265"/>
+      <c r="F26" s="275"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="265"/>
+      <c r="J26" s="275"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="265"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="280" t="s">
+      <c r="B29" s="282" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="281"/>
+      <c r="C29" s="283"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
@@ -6697,12 +6843,15 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -6716,15 +6865,12 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculating and interpreting valuation ratios
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF913AEC-599A-D548-8197-BF29CA93E3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B729ECBF-5528-AE44-B0A9-EF6CB0CB9EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="950" activeTab="5" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="950" activeTab="6" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -2039,40 +2039,46 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2081,23 +2087,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="274" t="s">
+      <c r="D5" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="274" t="s">
+      <c r="F5" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="275"/>
+      <c r="D6" s="265"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3264,19 +3264,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="274" t="s">
+      <c r="D14" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="274" t="s">
+      <c r="F14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="274" t="s">
+      <c r="H14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3289,15 +3289,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="275"/>
+      <c r="D15" s="265"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="275"/>
+      <c r="F15" s="265"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="275"/>
+      <c r="H15" s="265"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3475,16 +3475,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4051,7 +4051,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomRight" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4669,7 +4669,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4679,7 +4679,7 @@
         <f>'P&amp;L'!D11</f>
         <v>191504</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.5300408933626928</v>
@@ -4688,17 +4688,17 @@
         <f>'P&amp;L'!E11</f>
         <v>172829</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4706,15 +4706,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4725,7 +4725,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4735,7 +4735,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>48.472512323502379</v>
@@ -4744,17 +4744,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>53.570812768690445</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4762,15 +4762,15 @@
         <f>G5</f>
         <v>7.5300408933626928</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>6.813411653394307</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4781,7 +4781,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4791,7 +4791,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4800,17 +4800,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4818,15 +4818,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4837,7 +4837,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4847,7 +4847,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4856,17 +4856,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4874,15 +4874,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4893,7 +4893,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4903,7 +4903,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4912,12 +4912,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -4925,7 +4925,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -4933,15 +4933,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -4952,7 +4952,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -4962,7 +4962,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -4971,17 +4971,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="266" t="s">
+      <c r="M25" s="274" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -4989,15 +4989,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="267"/>
+      <c r="M26" s="275"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5008,34 +5008,34 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="42"/>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="44"/>
       <c r="I29" s="42"/>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="44"/>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="45"/>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5046,34 +5046,34 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="268" t="s">
+      <c r="B33" s="266" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="42"/>
-      <c r="F33" s="274"/>
+      <c r="F33" s="264"/>
       <c r="G33" s="44"/>
       <c r="I33" s="42"/>
-      <c r="J33" s="274"/>
+      <c r="J33" s="264"/>
       <c r="K33" s="44"/>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="269"/>
+      <c r="B34" s="267"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="45"/>
-      <c r="F34" s="275"/>
+      <c r="F34" s="265"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45"/>
-      <c r="J34" s="275"/>
+      <c r="J34" s="265"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5090,34 +5090,34 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="268" t="s">
+      <c r="B37" s="266" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="42"/>
-      <c r="F37" s="274"/>
+      <c r="F37" s="264"/>
       <c r="G37" s="44"/>
       <c r="I37" s="42"/>
-      <c r="J37" s="274"/>
+      <c r="J37" s="264"/>
       <c r="K37" s="44"/>
-      <c r="M37" s="264" t="s">
+      <c r="M37" s="268" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="269"/>
+      <c r="B38" s="267"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="45"/>
-      <c r="F38" s="275"/>
+      <c r="F38" s="265"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45"/>
-      <c r="J38" s="275"/>
+      <c r="J38" s="265"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="265"/>
+      <c r="M38" s="269"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5153,7 +5153,7 @@
         <f>I41+I43-I45</f>
         <v>68.548621585483062</v>
       </c>
-      <c r="M41" s="264" t="s">
+      <c r="M41" s="268" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5217,44 +5217,72 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="265"/>
+      <c r="M45" s="269"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="268" t="s">
+      <c r="B48" s="266" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="42"/>
-      <c r="F48" s="274"/>
+      <c r="F48" s="264"/>
       <c r="G48" s="44"/>
       <c r="I48" s="42"/>
-      <c r="J48" s="274"/>
+      <c r="J48" s="264"/>
       <c r="K48" s="44"/>
-      <c r="M48" s="264" t="s">
+      <c r="M48" s="268" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="269"/>
+      <c r="B49" s="267"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="45"/>
-      <c r="F49" s="275"/>
+      <c r="F49" s="265"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45"/>
-      <c r="J49" s="275"/>
+      <c r="J49" s="265"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="265"/>
+      <c r="M49" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F37:F38"/>
@@ -5271,34 +5299,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5357,7 +5357,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5368,7 +5368,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5377,17 +5377,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="266" t="s">
+      <c r="M5" s="274" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5396,18 +5396,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="267"/>
+      <c r="M6" s="275"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5418,7 +5418,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5427,17 +5427,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="266" t="s">
+      <c r="M9" s="274" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5446,18 +5446,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="267"/>
+      <c r="M10" s="275"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5468,7 +5468,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5477,17 +5477,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="266" t="s">
+      <c r="M13" s="274" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5496,18 +5496,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="267"/>
+      <c r="M14" s="275"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5518,7 +5518,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5527,17 +5527,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="266" t="s">
+      <c r="M17" s="274" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5546,27 +5546,18 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="267"/>
+      <c r="M18" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5577,6 +5568,15 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5635,7 +5635,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5646,7 +5646,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="66">
         <f>E5/E6</f>
         <v>0.2242426086824206</v>
@@ -5655,17 +5655,17 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
@@ -5674,15 +5674,15 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5701,7 +5701,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5712,7 +5712,7 @@
         <f>E5</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="66">
         <f>E9/E10</f>
         <v>0.18316843989261211</v>
@@ -5721,17 +5721,17 @@
         <f>I5</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
@@ -5740,15 +5740,15 @@
         <f>BS!D32+BS!D36+BS!D42</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>I6+I5</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5757,7 +5757,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5768,7 +5768,7 @@
         <f>E9</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="66">
         <f>E13/E14</f>
         <v>0.16262324749918616</v>
@@ -5777,17 +5777,17 @@
         <f>I9</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
@@ -5796,15 +5796,15 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5813,7 +5813,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5824,7 +5824,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="71">
         <f>E17/E18</f>
         <v>8.2755963302752313</v>
@@ -5833,17 +5833,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
@@ -5852,15 +5852,15 @@
         <f>'P&amp;L'!D26 * -1</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>'P&amp;L'!E26*-1</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -5869,7 +5869,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5880,7 +5880,7 @@
         <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="71">
         <f>E21/E22</f>
         <v>4.9604474630443471</v>
@@ -5889,17 +5889,17 @@
         <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
@@ -5908,21 +5908,21 @@
         <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -5933,7 +5933,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="71">
         <f>E25/E26</f>
         <v>1.4252956528831253</v>
@@ -5942,17 +5942,17 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
@@ -5961,28 +5961,25 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -5993,13 +5990,16 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6013,7 +6013,7 @@
   </sheetPr>
   <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -6065,7 +6065,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6076,7 +6076,7 @@
         <f>'P&amp;L'!D17</f>
         <v>48553.16</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="72">
         <f>E5/E6</f>
         <v>0.24417591591440571</v>
@@ -6085,17 +6085,17 @@
         <f>'P&amp;L'!E17</f>
         <v>41525.160000000003</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="72">
         <f>I5/I6</f>
         <v>0.23051476343530902</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
@@ -6104,15 +6104,15 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -6129,7 +6129,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6140,7 +6140,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="72">
         <f>E9/E10</f>
         <v>0.11340994241746086</v>
@@ -6149,17 +6149,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="72">
         <f>I9/I10</f>
         <v>0.1032357986244109</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
@@ -6168,15 +6168,15 @@
         <f>E6</f>
         <v>198845</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>I6</f>
         <v>180141</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6193,7 +6193,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6204,7 +6204,7 @@
         <f>'P&amp;L'!D28</f>
         <v>19826.000000000004</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="72">
         <f>E13/E14</f>
         <v>9.9705801000779526E-2</v>
@@ -6213,17 +6213,17 @@
         <f>'P&amp;L'!E28</f>
         <v>15605.000000000004</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="72">
         <f>I13/I14</f>
         <v>8.6626586951332588E-2</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
@@ -6232,18 +6232,18 @@
         <f>E10</f>
         <v>198845</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>I10</f>
         <v>180141</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6254,7 +6254,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="72">
         <f>E17/E18</f>
         <v>8.9003998088963782E-2</v>
@@ -6263,17 +6263,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="72">
         <f>I17/I18</f>
         <v>7.7505953669625482E-2</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
@@ -6282,18 +6282,18 @@
         <f>E14</f>
         <v>198845</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>I14</f>
         <v>180141</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6304,7 +6304,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="72">
         <f>E21/E22</f>
         <v>0.10127292131005892</v>
@@ -6313,17 +6313,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="72">
         <f>I21/I22</f>
         <v>8.4663592290410331E-2</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
@@ -6332,15 +6332,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6355,7 +6355,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6366,7 +6366,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="72">
         <f>E25/E26</f>
         <v>0.1290431488565453</v>
@@ -6375,17 +6375,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="72">
         <f>I25/I26</f>
         <v>0.11276957640916493</v>
       </c>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
@@ -6394,18 +6394,18 @@
         <f>E22</f>
         <v>174755.5</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>164911.5</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6416,7 +6416,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="72">
         <f>E29/E30</f>
         <v>0.14562655387297796</v>
@@ -6425,17 +6425,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="72">
         <f>I29/I30</f>
         <v>0.1276687765161397</v>
       </c>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
@@ -6444,18 +6444,18 @@
         <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
         <v>154855</v>
       </c>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E32:F32) + AVERAGE(BS!E36:F36) + AVERAGE(BS!E42:F42)</f>
         <v>145666</v>
       </c>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="276" t="s">
+      <c r="B33" s="278" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6466,7 +6466,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F33" s="278"/>
+      <c r="F33" s="276"/>
       <c r="G33" s="247">
         <f>E33/E34</f>
         <v>0.14434385449800183</v>
@@ -6476,17 +6476,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J33" s="278"/>
+      <c r="J33" s="276"/>
       <c r="K33" s="247">
         <f>I33/I34</f>
         <v>0.13136687601439562</v>
       </c>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="277"/>
+      <c r="B34" s="279"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
@@ -6495,22 +6495,45 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F34" s="279"/>
+      <c r="F34" s="277"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J34" s="279"/>
+      <c r="J34" s="277"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6523,29 +6546,6 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6559,7 +6559,9 @@
   </sheetPr>
   <dimension ref="B3:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6610,36 +6612,54 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>182</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="274"/>
-      <c r="G5" s="71"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="274"/>
-      <c r="K5" s="113"/>
-      <c r="M5" s="264" t="s">
+      <c r="E5" s="59">
+        <f>'P&amp;L'!D32</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F5" s="264"/>
+      <c r="G5" s="71">
+        <f>E5/E6</f>
+        <v>1.7698000000000003</v>
+      </c>
+      <c r="I5" s="59">
+        <f>'P&amp;L'!E32</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J5" s="264"/>
+      <c r="K5" s="113">
+        <f>I5/I6</f>
+        <v>1.3962000000000003</v>
+      </c>
+      <c r="M5" s="268" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="275"/>
+      <c r="E6" s="65">
+        <f>'P&amp;L'!D50</f>
+        <v>10000</v>
+      </c>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="275"/>
+      <c r="I6" s="65">
+        <f>E6</f>
+        <v>10000</v>
+      </c>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6660,38 +6680,56 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="116"/>
-      <c r="F9" s="274"/>
-      <c r="G9" s="71"/>
-      <c r="I9" s="196"/>
-      <c r="J9" s="278"/>
-      <c r="K9" s="197"/>
+      <c r="E9" s="116">
+        <f>'P&amp;L'!D53</f>
+        <v>2.95</v>
+      </c>
+      <c r="F9" s="264"/>
+      <c r="G9" s="71">
+        <f>E9/E10</f>
+        <v>1.6668550118657475</v>
+      </c>
+      <c r="I9" s="196">
+        <f>'P&amp;L'!E53</f>
+        <v>2.15</v>
+      </c>
+      <c r="J9" s="276"/>
+      <c r="K9" s="197">
+        <f>I9/I10</f>
+        <v>1.5398939979945563</v>
+      </c>
       <c r="L9" s="73"/>
-      <c r="M9" s="280" t="s">
+      <c r="M9" s="282" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="E10" s="117"/>
-      <c r="F10" s="275"/>
+      <c r="E10" s="117">
+        <f>G5</f>
+        <v>1.7698000000000003</v>
+      </c>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
-      <c r="I10" s="198"/>
-      <c r="J10" s="279"/>
+      <c r="I10" s="198">
+        <f>K5</f>
+        <v>1.3962000000000003</v>
+      </c>
+      <c r="J10" s="277"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="281"/>
+      <c r="M10" s="283"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6705,131 +6743,167 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="E13" s="119"/>
-      <c r="F13" s="274"/>
-      <c r="G13" s="71"/>
-      <c r="I13" s="119"/>
-      <c r="J13" s="274"/>
-      <c r="K13" s="113"/>
-      <c r="M13" s="264" t="s">
+      <c r="E13" s="119">
+        <f>'P&amp;L'!D54</f>
+        <v>29500</v>
+      </c>
+      <c r="F13" s="264"/>
+      <c r="G13" s="71">
+        <f>E13/E14</f>
+        <v>1.6668550118657472</v>
+      </c>
+      <c r="I13" s="119">
+        <f>'P&amp;L'!E54</f>
+        <v>21500</v>
+      </c>
+      <c r="J13" s="264"/>
+      <c r="K13" s="113">
+        <f>I13/I14</f>
+        <v>1.5398939979945563</v>
+      </c>
+      <c r="M13" s="268" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="120"/>
-      <c r="F14" s="275"/>
+      <c r="E14" s="120">
+        <f>'P&amp;L'!D32</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="275"/>
+      <c r="I14" s="120">
+        <f>'P&amp;L'!E32</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="116"/>
-      <c r="F17" s="274"/>
-      <c r="G17" s="250"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="274"/>
-      <c r="K17" s="250"/>
-      <c r="M17" s="264" t="s">
+      <c r="E17" s="116">
+        <f>'P&amp;L'!D51</f>
+        <v>0.88</v>
+      </c>
+      <c r="F17" s="264"/>
+      <c r="G17" s="250">
+        <f>E17/E18</f>
+        <v>0.29830508474576267</v>
+      </c>
+      <c r="I17" s="116">
+        <f>'P&amp;L'!E51</f>
+        <v>0.65</v>
+      </c>
+      <c r="J17" s="264"/>
+      <c r="K17" s="250">
+        <f>I17/I18</f>
+        <v>0.30232558139534887</v>
+      </c>
+      <c r="M17" s="268" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="275"/>
+      <c r="E18" s="117">
+        <f>'P&amp;L'!D53</f>
+        <v>2.95</v>
+      </c>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
-      <c r="I18" s="117"/>
-      <c r="J18" s="275"/>
+      <c r="I18" s="117">
+        <f>I9</f>
+        <v>2.15</v>
+      </c>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>199</v>
       </c>
       <c r="E21" s="42"/>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="66"/>
       <c r="I21" s="42"/>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="66"/>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E22" s="45"/>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45"/>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>204</v>
       </c>
       <c r="E25" s="42"/>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="66"/>
       <c r="I25" s="42"/>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="66"/>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
       <c r="E26" s="45"/>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45"/>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="282" t="s">
+      <c r="B29" s="280" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="283"/>
+      <c r="C29" s="281"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
@@ -6843,15 +6917,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -6865,12 +6936,15 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculating and interpreting DuPont model
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C226B2-788F-FF48-81B7-DD4A485C93B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB585E41-7DF7-C840-819F-631FA6963264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="950" activeTab="7" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="950" firstSheet="1" activeTab="6" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="281">
   <si>
     <t>Note</t>
   </si>
@@ -2039,40 +2039,46 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2081,23 +2087,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3133,8 +3133,8 @@
   </sheetPr>
   <dimension ref="B3:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="274" t="s">
+      <c r="D5" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="274" t="s">
+      <c r="F5" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="275"/>
+      <c r="D6" s="265"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3214,21 +3214,43 @@
       <c r="B8" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="86">
+        <f>E8*G8</f>
+        <v>0.1443438544980018</v>
+      </c>
       <c r="D8" s="80"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="96"/>
+      <c r="E8" s="100">
+        <f>'Profitability ratios'!G17</f>
+        <v>8.9003998088963782E-2</v>
+      </c>
+      <c r="F8" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="96">
+        <f>'Activity ratios'!G48</f>
+        <v>1.6217682081396296</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B9" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="87"/>
+      <c r="C9" s="87">
+        <f>E9*G9</f>
+        <v>0.13136687601439562</v>
+      </c>
       <c r="D9" s="58"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="97"/>
+      <c r="E9" s="101">
+        <f>'Profitability ratios'!K17</f>
+        <v>7.7505953669625482E-2</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="97">
+        <f>'Activity ratios'!K48</f>
+        <v>1.6949262578505397</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C11" s="3"/>
@@ -3264,19 +3286,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="274" t="s">
+      <c r="D14" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="274" t="s">
+      <c r="F14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="274" t="s">
+      <c r="H14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3289,15 +3311,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="275"/>
+      <c r="D15" s="265"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="275"/>
+      <c r="F15" s="265"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="275"/>
+      <c r="H15" s="265"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3310,26 +3332,58 @@
       <c r="B17" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="86"/>
+      <c r="C17" s="86">
+        <f>E17*G17*I17</f>
+        <v>0.1443438544980018</v>
+      </c>
       <c r="D17" s="80"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="96"/>
+      <c r="E17" s="100">
+        <f>E8</f>
+        <v>8.9003998088963782E-2</v>
+      </c>
+      <c r="F17" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="98">
+        <f>'Activity ratios'!G37</f>
+        <v>1.1378468774945567</v>
+      </c>
+      <c r="H17" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="96">
+        <f>'Solvency ratios'!G25</f>
+        <v>1.4252956528831253</v>
+      </c>
       <c r="J17" s="95"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B18" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="87"/>
+      <c r="C18" s="87">
+        <f>E18*G18*I18</f>
+        <v>0.13136687601439564</v>
+      </c>
       <c r="D18" s="58"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="97"/>
+      <c r="E18" s="101">
+        <f>E9</f>
+        <v>7.7505953669625482E-2</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="99">
+        <f>'Activity ratios'!K37</f>
+        <v>1.0923495329312995</v>
+      </c>
+      <c r="H18" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="97">
+        <f>'Solvency ratios'!K25</f>
+        <v>1.5516336179521557</v>
+      </c>
       <c r="J18" s="95"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
@@ -3447,15 +3501,30 @@
       </c>
       <c r="C26" s="86"/>
       <c r="D26" s="80"/>
-      <c r="E26" s="102"/>
+      <c r="E26" s="102">
+        <f>'P&amp;L'!D32/'P&amp;L'!D28</f>
+        <v>0.89266619590436802</v>
+      </c>
       <c r="F26" s="80"/>
-      <c r="G26" s="102"/>
+      <c r="G26" s="102">
+        <f>'P&amp;L'!D28/'P&amp;L'!D24</f>
+        <v>0.87916278657265756</v>
+      </c>
       <c r="H26" s="80"/>
-      <c r="I26" s="100"/>
+      <c r="I26" s="100">
+        <f>'Profitability ratios'!G9</f>
+        <v>0.11340994241746086</v>
+      </c>
       <c r="J26" s="80"/>
-      <c r="K26" s="98"/>
+      <c r="K26" s="98">
+        <f>G17</f>
+        <v>1.1378468774945567</v>
+      </c>
       <c r="L26" s="80"/>
-      <c r="M26" s="96"/>
+      <c r="M26" s="96">
+        <f>I17</f>
+        <v>1.4252956528831253</v>
+      </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B27" s="105" t="s">
@@ -3463,28 +3532,43 @@
       </c>
       <c r="C27" s="103"/>
       <c r="D27" s="58"/>
-      <c r="E27" s="104"/>
+      <c r="E27" s="104">
+        <f>'P&amp;L'!E32/'P&amp;L'!E28</f>
+        <v>0.89471323293816085</v>
+      </c>
       <c r="F27" s="58"/>
-      <c r="G27" s="104"/>
+      <c r="G27" s="104">
+        <f>'P&amp;L'!E28/'P&amp;L'!E24</f>
+        <v>0.83911383556487606</v>
+      </c>
       <c r="H27" s="58"/>
-      <c r="I27" s="101"/>
+      <c r="I27" s="101">
+        <f>'Profitability ratios'!K9</f>
+        <v>0.1032357986244109</v>
+      </c>
       <c r="J27" s="58"/>
-      <c r="K27" s="99"/>
+      <c r="K27" s="99">
+        <f>G18</f>
+        <v>1.0923495329312995</v>
+      </c>
       <c r="L27" s="58"/>
-      <c r="M27" s="97"/>
+      <c r="M27" s="97">
+        <f>I18</f>
+        <v>1.5516336179521557</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4669,7 +4753,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4679,7 +4763,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.8186929852154767</v>
@@ -4688,17 +4772,17 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4706,15 +4790,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4725,7 +4809,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4735,7 +4819,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>46.682994292036511</v>
@@ -4744,17 +4828,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>51.396350636445895</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4762,15 +4846,15 @@
         <f>G5</f>
         <v>7.8186929852154767</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4781,7 +4865,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4791,7 +4875,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4800,17 +4884,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4818,15 +4902,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4837,7 +4921,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4847,7 +4931,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4856,17 +4940,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4874,15 +4958,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4893,7 +4977,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4903,7 +4987,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4912,12 +4996,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -4925,7 +5009,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -4933,15 +5017,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -4952,7 +5036,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -4962,7 +5046,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -4971,17 +5055,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="266" t="s">
+      <c r="M25" s="274" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -4989,15 +5073,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="267"/>
+      <c r="M26" s="275"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5008,7 +5092,7 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -5018,7 +5102,7 @@
         <f>E5</f>
         <v>198845</v>
       </c>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="44">
         <f>E29/E30</f>
         <v>1.8745787159025025</v>
@@ -5027,17 +5111,17 @@
         <f>I5</f>
         <v>180141</v>
       </c>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="44">
         <f>I29/I30</f>
         <v>1.72279045747321</v>
       </c>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
@@ -5045,15 +5129,15 @@
         <f>AVERAGE(BS!D11:E11)</f>
         <v>106074.5</v>
       </c>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E11:F11)</f>
         <v>104563.5</v>
       </c>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5064,7 +5148,7 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="268" t="s">
+      <c r="B33" s="266" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
@@ -5074,7 +5158,7 @@
         <f>E29</f>
         <v>198845</v>
       </c>
-      <c r="F33" s="274"/>
+      <c r="F33" s="264"/>
       <c r="G33" s="44">
         <f>E33/E34</f>
         <v>5.8375656871091799</v>
@@ -5083,17 +5167,17 @@
         <f>I29</f>
         <v>180141</v>
       </c>
-      <c r="J33" s="274"/>
+      <c r="J33" s="264"/>
       <c r="K33" s="44">
         <f>I33/I34</f>
         <v>7.4487677803506447</v>
       </c>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="269"/>
+      <c r="B34" s="267"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
@@ -5101,15 +5185,15 @@
         <f>AVERAGE(BS!D22:E22) - AVERAGE(BS!D45:E45)</f>
         <v>34063</v>
       </c>
-      <c r="F34" s="275"/>
+      <c r="F34" s="265"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45">
         <f>AVERAGE(BS!E22:F22)-AVERAGE(BS!E45:F45)</f>
         <v>24184</v>
       </c>
-      <c r="J34" s="275"/>
+      <c r="J34" s="265"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5126,7 +5210,7 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="268" t="s">
+      <c r="B37" s="266" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
@@ -5136,7 +5220,7 @@
         <f>E33</f>
         <v>198845</v>
       </c>
-      <c r="F37" s="274"/>
+      <c r="F37" s="264"/>
       <c r="G37" s="44">
         <f>E37/E38</f>
         <v>1.1378468774945567</v>
@@ -5145,17 +5229,17 @@
         <f>I33</f>
         <v>180141</v>
       </c>
-      <c r="J37" s="274"/>
+      <c r="J37" s="264"/>
       <c r="K37" s="44">
         <f>I37/I38</f>
         <v>1.0923495329312995</v>
       </c>
-      <c r="M37" s="264" t="s">
+      <c r="M37" s="268" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="269"/>
+      <c r="B38" s="267"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
@@ -5163,15 +5247,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F38" s="275"/>
+      <c r="F38" s="265"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J38" s="275"/>
+      <c r="J38" s="265"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="265"/>
+      <c r="M38" s="269"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5207,7 +5291,7 @@
         <f>I41+I43-I45</f>
         <v>66.374159453238519</v>
       </c>
-      <c r="M41" s="264" t="s">
+      <c r="M41" s="268" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5271,14 +5355,14 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="265"/>
+      <c r="M45" s="269"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="268" t="s">
+      <c r="B48" s="266" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
@@ -5288,7 +5372,7 @@
         <f>E37</f>
         <v>198845</v>
       </c>
-      <c r="F48" s="274"/>
+      <c r="F48" s="264"/>
       <c r="G48" s="44">
         <f>E48/E49</f>
         <v>1.6217682081396296</v>
@@ -5297,17 +5381,17 @@
         <f>I37</f>
         <v>180141</v>
       </c>
-      <c r="J48" s="274"/>
+      <c r="J48" s="264"/>
       <c r="K48" s="44">
         <f>I48/I49</f>
         <v>1.6949262578505397</v>
       </c>
-      <c r="M48" s="264" t="s">
+      <c r="M48" s="268" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="269"/>
+      <c r="B49" s="267"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
@@ -5315,18 +5399,46 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F49" s="275"/>
+      <c r="F49" s="265"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J49" s="275"/>
+      <c r="J49" s="265"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="265"/>
+      <c r="M49" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F37:F38"/>
@@ -5343,34 +5455,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5429,7 +5513,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5440,7 +5524,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5449,17 +5533,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="266" t="s">
+      <c r="M5" s="274" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5468,18 +5552,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="267"/>
+      <c r="M6" s="275"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5490,7 +5574,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5499,17 +5583,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="266" t="s">
+      <c r="M9" s="274" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5518,18 +5602,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="267"/>
+      <c r="M10" s="275"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5540,7 +5624,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5549,17 +5633,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="266" t="s">
+      <c r="M13" s="274" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5568,18 +5652,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="267"/>
+      <c r="M14" s="275"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5590,7 +5674,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5599,17 +5683,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="266" t="s">
+      <c r="M17" s="274" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5618,27 +5702,18 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="267"/>
+      <c r="M18" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5649,6 +5724,15 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5707,7 +5791,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5718,7 +5802,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="66">
         <f>E5/E6</f>
         <v>0.2242426086824206</v>
@@ -5727,17 +5811,17 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
@@ -5746,15 +5830,15 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5773,7 +5857,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5784,7 +5868,7 @@
         <f>E5</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="66">
         <f>E9/E10</f>
         <v>0.18316843989261211</v>
@@ -5793,17 +5877,17 @@
         <f>I5</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
@@ -5812,15 +5896,15 @@
         <f>BS!D32+BS!D36+BS!D42</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>I6+I5</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5829,7 +5913,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5840,7 +5924,7 @@
         <f>E9</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="66">
         <f>E13/E14</f>
         <v>0.16262324749918616</v>
@@ -5849,17 +5933,17 @@
         <f>I9</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
@@ -5868,15 +5952,15 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5885,7 +5969,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5896,7 +5980,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="71">
         <f>E17/E18</f>
         <v>8.2755963302752313</v>
@@ -5905,17 +5989,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
@@ -5924,15 +6008,15 @@
         <f>'P&amp;L'!D26 * -1</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>'P&amp;L'!E26*-1</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -5941,7 +6025,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5952,7 +6036,7 @@
         <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="71">
         <f>E21/E22</f>
         <v>4.9604474630443471</v>
@@ -5961,17 +6045,17 @@
         <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
@@ -5980,21 +6064,21 @@
         <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6005,7 +6089,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="71">
         <f>E25/E26</f>
         <v>1.4252956528831253</v>
@@ -6014,17 +6098,17 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
@@ -6033,28 +6117,25 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -6065,13 +6146,16 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6137,7 +6221,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6148,7 +6232,7 @@
         <f>'P&amp;L'!D17</f>
         <v>48553.16</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="72">
         <f>E5/E6</f>
         <v>0.24417591591440571</v>
@@ -6157,17 +6241,17 @@
         <f>'P&amp;L'!E17</f>
         <v>41525.160000000003</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="72">
         <f>I5/I6</f>
         <v>0.23051476343530902</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
@@ -6176,15 +6260,15 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -6201,7 +6285,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6212,7 +6296,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="72">
         <f>E9/E10</f>
         <v>0.11340994241746086</v>
@@ -6221,17 +6305,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J9" s="274"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="72">
         <f>I9/I10</f>
         <v>0.1032357986244109</v>
       </c>
-      <c r="M9" s="264" t="s">
+      <c r="M9" s="268" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
@@ -6240,15 +6324,15 @@
         <f>E6</f>
         <v>198845</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>I6</f>
         <v>180141</v>
       </c>
-      <c r="J10" s="275"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="265"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6265,7 +6349,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6276,7 +6360,7 @@
         <f>'P&amp;L'!D28</f>
         <v>19826.000000000004</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="72">
         <f>E13/E14</f>
         <v>9.9705801000779526E-2</v>
@@ -6285,17 +6369,17 @@
         <f>'P&amp;L'!E28</f>
         <v>15605.000000000004</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="72">
         <f>I13/I14</f>
         <v>8.6626586951332588E-2</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
@@ -6304,18 +6388,18 @@
         <f>E10</f>
         <v>198845</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>I10</f>
         <v>180141</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6326,7 +6410,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="72">
         <f>E17/E18</f>
         <v>8.9003998088963782E-2</v>
@@ -6335,17 +6419,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="72">
         <f>I17/I18</f>
         <v>7.7505953669625482E-2</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
@@ -6354,18 +6438,18 @@
         <f>E14</f>
         <v>198845</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>I14</f>
         <v>180141</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6376,7 +6460,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F21" s="274"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="72">
         <f>E21/E22</f>
         <v>0.10127292131005892</v>
@@ -6385,17 +6469,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J21" s="274"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="72">
         <f>I21/I22</f>
         <v>8.4663592290410331E-2</v>
       </c>
-      <c r="M21" s="264" t="s">
+      <c r="M21" s="268" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
@@ -6404,15 +6488,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F22" s="275"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J22" s="275"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6427,7 +6511,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6438,7 +6522,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F25" s="274"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="72">
         <f>E25/E26</f>
         <v>0.1290431488565453</v>
@@ -6447,17 +6531,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J25" s="274"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="72">
         <f>I25/I26</f>
         <v>0.11276957640916493</v>
       </c>
-      <c r="M25" s="264" t="s">
+      <c r="M25" s="268" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
@@ -6466,18 +6550,18 @@
         <f>E22</f>
         <v>174755.5</v>
       </c>
-      <c r="F26" s="275"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>164911.5</v>
       </c>
-      <c r="J26" s="275"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="268" t="s">
+      <c r="B29" s="266" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6488,7 +6572,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F29" s="274"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="72">
         <f>E29/E30</f>
         <v>0.14562655387297796</v>
@@ -6497,17 +6581,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J29" s="274"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="72">
         <f>I29/I30</f>
         <v>0.1276687765161397</v>
       </c>
-      <c r="M29" s="264" t="s">
+      <c r="M29" s="268" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="269"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
@@ -6516,18 +6600,18 @@
         <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
         <v>154855</v>
       </c>
-      <c r="F30" s="275"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E32:F32) + AVERAGE(BS!E36:F36) + AVERAGE(BS!E42:F42)</f>
         <v>145666</v>
       </c>
-      <c r="J30" s="275"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="265"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="276" t="s">
+      <c r="B33" s="278" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6538,7 +6622,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F33" s="278"/>
+      <c r="F33" s="276"/>
       <c r="G33" s="247">
         <f>E33/E34</f>
         <v>0.14434385449800183</v>
@@ -6548,17 +6632,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J33" s="278"/>
+      <c r="J33" s="276"/>
       <c r="K33" s="247">
         <f>I33/I34</f>
         <v>0.13136687601439562</v>
       </c>
-      <c r="M33" s="264" t="s">
+      <c r="M33" s="268" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="277"/>
+      <c r="B34" s="279"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
@@ -6567,22 +6651,45 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F34" s="279"/>
+      <c r="F34" s="277"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J34" s="279"/>
+      <c r="J34" s="277"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="265"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6595,29 +6702,6 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6631,8 +6715,8 @@
   </sheetPr>
   <dimension ref="B3:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -6684,7 +6768,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="268" t="s">
+      <c r="B5" s="266" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6695,7 +6779,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F5" s="274"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="71">
         <f>E5/E6</f>
         <v>1.7698000000000003</v>
@@ -6704,17 +6788,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J5" s="274"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="113">
         <f>I5/I6</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="M5" s="264" t="s">
+      <c r="M5" s="268" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="269"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
@@ -6723,15 +6807,15 @@
         <f>'P&amp;L'!D50</f>
         <v>10000</v>
       </c>
-      <c r="F6" s="275"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>E6</f>
         <v>10000</v>
       </c>
-      <c r="J6" s="275"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="265"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6752,7 +6836,7 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="268" t="s">
+      <c r="B9" s="266" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6762,7 +6846,7 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="71">
         <f>E9/E10</f>
         <v>1.6668550118657475</v>
@@ -6771,20 +6855,20 @@
         <f>'P&amp;L'!E53</f>
         <v>2.15</v>
       </c>
-      <c r="J9" s="278"/>
+      <c r="J9" s="276"/>
       <c r="K9" s="197">
         <f>I9/I10</f>
         <v>1.5398939979945563</v>
       </c>
       <c r="L9" s="73"/>
-      <c r="M9" s="280" t="s">
+      <c r="M9" s="282" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="269"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
@@ -6792,16 +6876,16 @@
         <f>G5</f>
         <v>1.7698000000000003</v>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198">
         <f>K5</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="J10" s="279"/>
+      <c r="J10" s="277"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="281"/>
+      <c r="M10" s="283"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6815,7 +6899,7 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="268" t="s">
+      <c r="B13" s="266" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6825,7 +6909,7 @@
         <f>'P&amp;L'!D54</f>
         <v>29500</v>
       </c>
-      <c r="F13" s="274"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="71">
         <f>E13/E14</f>
         <v>1.6668550118657472</v>
@@ -6834,17 +6918,17 @@
         <f>'P&amp;L'!E54</f>
         <v>21500</v>
       </c>
-      <c r="J13" s="274"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="113">
         <f>I13/I14</f>
         <v>1.5398939979945563</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="268" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="269"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
@@ -6852,18 +6936,18 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F14" s="275"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J14" s="275"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="265"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="268" t="s">
+      <c r="B17" s="266" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6873,7 +6957,7 @@
         <f>'P&amp;L'!D51</f>
         <v>0.88</v>
       </c>
-      <c r="F17" s="274"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="250">
         <f>E17/E18</f>
         <v>0.29830508474576267</v>
@@ -6882,17 +6966,17 @@
         <f>'P&amp;L'!E51</f>
         <v>0.65</v>
       </c>
-      <c r="J17" s="274"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="250">
         <f>I17/I18</f>
         <v>0.30232558139534887</v>
       </c>
-      <c r="M17" s="264" t="s">
+      <c r="M17" s="268" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="269"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
@@ -6900,82 +6984,118 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F18" s="275"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117">
         <f>I9</f>
         <v>2.15</v>
       </c>
-      <c r="J18" s="275"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="265"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="268" t="s">
+      <c r="B21" s="266" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="274"/>
-      <c r="G21" s="66"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="274"/>
-      <c r="K21" s="66"/>
-      <c r="M21" s="264" t="s">
+      <c r="E21" s="42">
+        <f>'P&amp;L'!D32-'P&amp;L'!D52</f>
+        <v>8898.0000000000036</v>
+      </c>
+      <c r="F21" s="264"/>
+      <c r="G21" s="66">
+        <f>E21/E22</f>
+        <v>0.50276867442648898</v>
+      </c>
+      <c r="I21" s="42">
+        <f>'P&amp;L'!E32-'P&amp;L'!E52</f>
+        <v>7462.0000000000036</v>
+      </c>
+      <c r="J21" s="264"/>
+      <c r="K21" s="66">
+        <f>I21/I22</f>
+        <v>0.53445065176908768</v>
+      </c>
+      <c r="M21" s="268" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="269"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="275"/>
+      <c r="E22" s="45">
+        <f>E14</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="275"/>
+      <c r="I22" s="45">
+        <f>I14</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="265"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="268" t="s">
+      <c r="B25" s="266" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="274"/>
-      <c r="G25" s="66"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="274"/>
-      <c r="K25" s="66"/>
-      <c r="M25" s="264" t="s">
+      <c r="E25" s="42">
+        <f>'P&amp;L'!D52</f>
+        <v>8800</v>
+      </c>
+      <c r="F25" s="264"/>
+      <c r="G25" s="66">
+        <f>E25/E26</f>
+        <v>0.49723132557351102</v>
+      </c>
+      <c r="I25" s="42">
+        <f>'P&amp;L'!E52</f>
+        <v>6500</v>
+      </c>
+      <c r="J25" s="264"/>
+      <c r="K25" s="66">
+        <f>I25/I26</f>
+        <v>0.46554934823091237</v>
+      </c>
+      <c r="M25" s="268" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="269"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="275"/>
+      <c r="E26" s="45">
+        <f>E22</f>
+        <v>17698.000000000004</v>
+      </c>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="275"/>
+      <c r="I26" s="45">
+        <f>I22</f>
+        <v>13962.000000000004</v>
+      </c>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="265"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="282" t="s">
+      <c r="B29" s="280" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="283"/>
+      <c r="C29" s="281"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
@@ -6989,15 +7109,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -7011,12 +7128,15 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7030,7 +7150,7 @@
   </sheetPr>
   <dimension ref="B1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -7500,7 +7620,7 @@
   </sheetPr>
   <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Calculating and interpreting sustainable growth rate
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB585E41-7DF7-C840-819F-631FA6963264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E08BA-63A9-034E-AF7D-AE10FA6A4AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="950" firstSheet="1" activeTab="6" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
@@ -2028,7 +2028,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2039,41 +2038,47 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2081,11 +2086,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2093,12 +2098,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2150,6 +2149,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2889,17 +2889,17 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="6"/>
-      <c r="C33" s="261"/>
-      <c r="D33" s="262"/>
-      <c r="E33" s="262"/>
+      <c r="C33" s="260"/>
+      <c r="D33" s="261"/>
+      <c r="E33" s="261"/>
     </row>
     <row r="34" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="261"/>
-      <c r="D34" s="263"/>
-      <c r="E34" s="263"/>
+      <c r="C34" s="260"/>
+      <c r="D34" s="262"/>
+      <c r="E34" s="262"/>
     </row>
     <row r="35" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="273" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="264" t="s">
+      <c r="F5" s="273" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="265"/>
+      <c r="D6" s="274"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3286,19 +3286,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="264" t="s">
+      <c r="D14" s="273" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="264" t="s">
+      <c r="F14" s="273" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="264" t="s">
+      <c r="H14" s="273" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3311,15 +3311,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="265"/>
+      <c r="D15" s="274"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="265"/>
+      <c r="F15" s="274"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="265"/>
+      <c r="H15" s="274"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3428,31 +3428,31 @@
       <c r="C23" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="292" t="s">
+      <c r="D23" s="291" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="292" t="s">
+      <c r="F23" s="291" t="s">
         <v>97</v>
       </c>
       <c r="G23" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="292" t="s">
+      <c r="H23" s="291" t="s">
         <v>97</v>
       </c>
       <c r="I23" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="292" t="s">
+      <c r="J23" s="291" t="s">
         <v>97</v>
       </c>
       <c r="K23" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="292" t="s">
+      <c r="L23" s="291" t="s">
         <v>97</v>
       </c>
       <c r="M23" s="90" t="s">
@@ -3463,23 +3463,23 @@
       <c r="C24" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="293"/>
+      <c r="D24" s="292"/>
       <c r="E24" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="293"/>
+      <c r="F24" s="292"/>
       <c r="G24" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="293"/>
+      <c r="H24" s="292"/>
       <c r="I24" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="293"/>
+      <c r="J24" s="292"/>
       <c r="K24" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="293"/>
+      <c r="L24" s="292"/>
       <c r="M24" s="93" t="s">
         <v>94</v>
       </c>
@@ -3559,16 +3559,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="J23:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3599,14 +3599,14 @@
   <sheetData>
     <row r="2" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="294" t="s">
+      <c r="D3" s="293" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="295"/>
-      <c r="F3" s="296" t="s">
+      <c r="E3" s="294"/>
+      <c r="F3" s="295" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="297"/>
+      <c r="G3" s="296"/>
     </row>
     <row r="4" spans="2:14" s="142" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="251" t="s">
@@ -3754,16 +3754,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="C3" s="298" t="s">
+      <c r="C3" s="297" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="299"/>
-      <c r="E3" s="299"/>
-      <c r="F3" s="298" t="s">
+      <c r="D3" s="298"/>
+      <c r="E3" s="298"/>
+      <c r="F3" s="297" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="299"/>
-      <c r="H3" s="300"/>
+      <c r="G3" s="298"/>
+      <c r="H3" s="299"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B4" s="142"/>
@@ -3976,16 +3976,16 @@
       <c r="G11" s="139"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="C13" s="298" t="s">
+      <c r="C13" s="297" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="299"/>
-      <c r="E13" s="300"/>
-      <c r="F13" s="298" t="s">
+      <c r="D13" s="298"/>
+      <c r="E13" s="299"/>
+      <c r="F13" s="297" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="299"/>
-      <c r="H13" s="300"/>
+      <c r="G13" s="298"/>
+      <c r="H13" s="299"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C14" s="255" t="s">
@@ -4730,22 +4730,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="270"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="270" t="s">
+      <c r="E3" s="269" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="269" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="272"/>
-      <c r="K3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -4753,7 +4753,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="267" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4763,7 +4763,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="273"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.8186929852154767</v>
@@ -4772,17 +4772,17 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="273"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="263" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="268"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4790,15 +4790,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="274"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="264"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4809,7 +4809,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="267" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4819,7 +4819,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="273"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>46.682994292036511</v>
@@ -4828,17 +4828,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="273"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>51.396350636445895</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="263" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="268"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4846,15 +4846,15 @@
         <f>G5</f>
         <v>7.8186929852154767</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="274"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="274"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="264"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4865,7 +4865,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="267" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4875,7 +4875,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="273"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4884,17 +4884,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="273"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="263" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="268"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4902,15 +4902,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="274"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="274"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="264"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4921,7 +4921,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="267" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4931,7 +4931,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4940,17 +4940,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="273"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="263" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="268"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4958,15 +4958,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="274"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="274"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="264"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4977,7 +4977,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="267" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4987,7 +4987,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="273"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4996,12 +4996,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="273"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="263" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -5009,7 +5009,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="268"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -5017,15 +5017,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="274"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="274"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="264"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -5036,7 +5036,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="267" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -5046,7 +5046,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="273"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -5055,17 +5055,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="273"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="274" t="s">
+      <c r="M25" s="265" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="268"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -5073,15 +5073,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="274"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="274"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="275"/>
+      <c r="M26" s="266"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5092,7 +5092,7 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="267" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -5102,7 +5102,7 @@
         <f>E5</f>
         <v>198845</v>
       </c>
-      <c r="F29" s="264"/>
+      <c r="F29" s="273"/>
       <c r="G29" s="44">
         <f>E29/E30</f>
         <v>1.8745787159025025</v>
@@ -5111,17 +5111,17 @@
         <f>I5</f>
         <v>180141</v>
       </c>
-      <c r="J29" s="264"/>
+      <c r="J29" s="273"/>
       <c r="K29" s="44">
         <f>I29/I30</f>
         <v>1.72279045747321</v>
       </c>
-      <c r="M29" s="268" t="s">
+      <c r="M29" s="263" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="268"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
@@ -5129,15 +5129,15 @@
         <f>AVERAGE(BS!D11:E11)</f>
         <v>106074.5</v>
       </c>
-      <c r="F30" s="265"/>
+      <c r="F30" s="274"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E11:F11)</f>
         <v>104563.5</v>
       </c>
-      <c r="J30" s="265"/>
+      <c r="J30" s="274"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="264"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5148,7 +5148,7 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="266" t="s">
+      <c r="B33" s="267" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
@@ -5158,7 +5158,7 @@
         <f>E29</f>
         <v>198845</v>
       </c>
-      <c r="F33" s="264"/>
+      <c r="F33" s="273"/>
       <c r="G33" s="44">
         <f>E33/E34</f>
         <v>5.8375656871091799</v>
@@ -5167,17 +5167,17 @@
         <f>I29</f>
         <v>180141</v>
       </c>
-      <c r="J33" s="264"/>
+      <c r="J33" s="273"/>
       <c r="K33" s="44">
         <f>I33/I34</f>
         <v>7.4487677803506447</v>
       </c>
-      <c r="M33" s="268" t="s">
+      <c r="M33" s="263" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="267"/>
+      <c r="B34" s="268"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
@@ -5185,15 +5185,15 @@
         <f>AVERAGE(BS!D22:E22) - AVERAGE(BS!D45:E45)</f>
         <v>34063</v>
       </c>
-      <c r="F34" s="265"/>
+      <c r="F34" s="274"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45">
         <f>AVERAGE(BS!E22:F22)-AVERAGE(BS!E45:F45)</f>
         <v>24184</v>
       </c>
-      <c r="J34" s="265"/>
+      <c r="J34" s="274"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="264"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5210,7 +5210,7 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="266" t="s">
+      <c r="B37" s="267" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
@@ -5220,7 +5220,7 @@
         <f>E33</f>
         <v>198845</v>
       </c>
-      <c r="F37" s="264"/>
+      <c r="F37" s="273"/>
       <c r="G37" s="44">
         <f>E37/E38</f>
         <v>1.1378468774945567</v>
@@ -5229,17 +5229,17 @@
         <f>I33</f>
         <v>180141</v>
       </c>
-      <c r="J37" s="264"/>
+      <c r="J37" s="273"/>
       <c r="K37" s="44">
         <f>I37/I38</f>
         <v>1.0923495329312995</v>
       </c>
-      <c r="M37" s="268" t="s">
+      <c r="M37" s="263" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="267"/>
+      <c r="B38" s="268"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
@@ -5247,15 +5247,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F38" s="265"/>
+      <c r="F38" s="274"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J38" s="265"/>
+      <c r="J38" s="274"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="269"/>
+      <c r="M38" s="264"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5291,7 +5291,7 @@
         <f>I41+I43-I45</f>
         <v>66.374159453238519</v>
       </c>
-      <c r="M41" s="268" t="s">
+      <c r="M41" s="263" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5305,7 +5305,7 @@
       <c r="I42" s="54"/>
       <c r="J42" s="35"/>
       <c r="K42" s="50"/>
-      <c r="M42" s="273"/>
+      <c r="M42" s="272"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B43" s="49"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="50"/>
-      <c r="M43" s="273"/>
+      <c r="M43" s="272"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B44" s="49"/>
@@ -5336,7 +5336,7 @@
       <c r="I44" s="54"/>
       <c r="J44" s="56"/>
       <c r="K44" s="50"/>
-      <c r="M44" s="273"/>
+      <c r="M44" s="272"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B45" s="51"/>
@@ -5355,14 +5355,14 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="269"/>
+      <c r="M45" s="264"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="266" t="s">
+      <c r="B48" s="267" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
@@ -5372,7 +5372,7 @@
         <f>E37</f>
         <v>198845</v>
       </c>
-      <c r="F48" s="264"/>
+      <c r="F48" s="273"/>
       <c r="G48" s="44">
         <f>E48/E49</f>
         <v>1.6217682081396296</v>
@@ -5381,17 +5381,17 @@
         <f>I37</f>
         <v>180141</v>
       </c>
-      <c r="J48" s="264"/>
+      <c r="J48" s="273"/>
       <c r="K48" s="44">
         <f>I48/I49</f>
         <v>1.6949262578505397</v>
       </c>
-      <c r="M48" s="268" t="s">
+      <c r="M48" s="263" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="267"/>
+      <c r="B49" s="268"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
@@ -5399,25 +5399,39 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F49" s="265"/>
+      <c r="F49" s="274"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J49" s="265"/>
+      <c r="J49" s="274"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="269"/>
+      <c r="M49" s="264"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="M37:M38"/>
@@ -5434,27 +5448,13 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="M41:M45"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5491,29 +5491,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="270"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="270" t="s">
+      <c r="E3" s="269" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="269" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="272"/>
-      <c r="K3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="267" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5524,7 +5524,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="273"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5533,17 +5533,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="273"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="274" t="s">
+      <c r="M5" s="265" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="268"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5552,18 +5552,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="274"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="275"/>
+      <c r="M6" s="266"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="267" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5574,7 +5574,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="273"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5583,17 +5583,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="273"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="274" t="s">
+      <c r="M9" s="265" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="268"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5602,18 +5602,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="274"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="274"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="275"/>
+      <c r="M10" s="266"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="267" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5624,7 +5624,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="273"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5633,17 +5633,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="273"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="274" t="s">
+      <c r="M13" s="265" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="268"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5652,18 +5652,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="274"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="274"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="275"/>
+      <c r="M14" s="266"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="267" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5674,7 +5674,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5683,17 +5683,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="273"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="274" t="s">
+      <c r="M17" s="265" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="268"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5702,18 +5702,27 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="274"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="274"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="275"/>
+      <c r="M18" s="266"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5724,15 +5733,6 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5769,29 +5769,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="270"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="270" t="s">
+      <c r="E3" s="269" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="269" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="272"/>
-      <c r="K3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="267" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5802,7 +5802,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="273"/>
       <c r="G5" s="66">
         <f>E5/E6</f>
         <v>0.2242426086824206</v>
@@ -5811,17 +5811,17 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="273"/>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="263" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="268"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
@@ -5830,15 +5830,15 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="274"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="264"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5857,7 +5857,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="267" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5868,7 +5868,7 @@
         <f>E5</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="273"/>
       <c r="G9" s="66">
         <f>E9/E10</f>
         <v>0.18316843989261211</v>
@@ -5877,17 +5877,17 @@
         <f>I5</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="273"/>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="263" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="268"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
@@ -5896,15 +5896,15 @@
         <f>BS!D32+BS!D36+BS!D42</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="274"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>I6+I5</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="274"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="264"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5913,7 +5913,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="267" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5924,7 +5924,7 @@
         <f>E9</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="273"/>
       <c r="G13" s="66">
         <f>E13/E14</f>
         <v>0.16262324749918616</v>
@@ -5933,17 +5933,17 @@
         <f>I9</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="273"/>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="263" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="268"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
@@ -5952,15 +5952,15 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="274"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="274"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="264"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5969,7 +5969,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="267" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5980,7 +5980,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="71">
         <f>E17/E18</f>
         <v>8.2755963302752313</v>
@@ -5989,17 +5989,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="273"/>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="263" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="268"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
@@ -6008,15 +6008,15 @@
         <f>'P&amp;L'!D26 * -1</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="274"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>'P&amp;L'!E26*-1</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="274"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="264"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -6025,7 +6025,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="267" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6036,7 +6036,7 @@
         <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="273"/>
       <c r="G21" s="71">
         <f>E21/E22</f>
         <v>4.9604474630443471</v>
@@ -6045,17 +6045,17 @@
         <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="273"/>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="263" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="268"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
@@ -6064,21 +6064,21 @@
         <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="274"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="274"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="264"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="267" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6089,7 +6089,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="273"/>
       <c r="G25" s="71">
         <f>E25/E26</f>
         <v>1.4252956528831253</v>
@@ -6098,17 +6098,17 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="273"/>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="263" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="268"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
@@ -6117,25 +6117,28 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="274"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="274"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="264"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -6146,16 +6149,13 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6192,22 +6192,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="270"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="270" t="s">
+      <c r="E3" s="269" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="269" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="272"/>
-      <c r="K3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -6221,7 +6221,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="267" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6232,7 +6232,7 @@
         <f>'P&amp;L'!D17</f>
         <v>48553.16</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="273"/>
       <c r="G5" s="72">
         <f>E5/E6</f>
         <v>0.24417591591440571</v>
@@ -6241,17 +6241,17 @@
         <f>'P&amp;L'!E17</f>
         <v>41525.160000000003</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="273"/>
       <c r="K5" s="72">
         <f>I5/I6</f>
         <v>0.23051476343530902</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="263" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="268"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
@@ -6260,15 +6260,15 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="274"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="264"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -6285,7 +6285,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="267" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6296,7 +6296,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="273"/>
       <c r="G9" s="72">
         <f>E9/E10</f>
         <v>0.11340994241746086</v>
@@ -6305,17 +6305,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J9" s="264"/>
+      <c r="J9" s="273"/>
       <c r="K9" s="72">
         <f>I9/I10</f>
         <v>0.1032357986244109</v>
       </c>
-      <c r="M9" s="268" t="s">
+      <c r="M9" s="263" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="268"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
@@ -6324,15 +6324,15 @@
         <f>E6</f>
         <v>198845</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="274"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>I6</f>
         <v>180141</v>
       </c>
-      <c r="J10" s="265"/>
+      <c r="J10" s="274"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="269"/>
+      <c r="M10" s="264"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6349,7 +6349,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="267" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6360,7 +6360,7 @@
         <f>'P&amp;L'!D28</f>
         <v>19826.000000000004</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="273"/>
       <c r="G13" s="72">
         <f>E13/E14</f>
         <v>9.9705801000779526E-2</v>
@@ -6369,17 +6369,17 @@
         <f>'P&amp;L'!E28</f>
         <v>15605.000000000004</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="273"/>
       <c r="K13" s="72">
         <f>I13/I14</f>
         <v>8.6626586951332588E-2</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="263" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="268"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
@@ -6388,18 +6388,18 @@
         <f>E10</f>
         <v>198845</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="274"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>I10</f>
         <v>180141</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="274"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="264"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="267" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6410,7 +6410,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="72">
         <f>E17/E18</f>
         <v>8.9003998088963782E-2</v>
@@ -6419,17 +6419,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="273"/>
       <c r="K17" s="72">
         <f>I17/I18</f>
         <v>7.7505953669625482E-2</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="263" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="268"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
@@ -6438,18 +6438,18 @@
         <f>E14</f>
         <v>198845</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="274"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>I14</f>
         <v>180141</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="274"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="264"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="267" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6460,7 +6460,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="273"/>
       <c r="G21" s="72">
         <f>E21/E22</f>
         <v>0.10127292131005892</v>
@@ -6469,17 +6469,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="273"/>
       <c r="K21" s="72">
         <f>I21/I22</f>
         <v>8.4663592290410331E-2</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="263" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="268"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
@@ -6488,15 +6488,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="274"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="274"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="264"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6511,7 +6511,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="267" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6522,7 +6522,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="273"/>
       <c r="G25" s="72">
         <f>E25/E26</f>
         <v>0.1290431488565453</v>
@@ -6531,17 +6531,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="273"/>
       <c r="K25" s="72">
         <f>I25/I26</f>
         <v>0.11276957640916493</v>
       </c>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="263" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="268"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
@@ -6550,18 +6550,18 @@
         <f>E22</f>
         <v>174755.5</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="274"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>164911.5</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="274"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="264"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="266" t="s">
+      <c r="B29" s="267" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6572,7 +6572,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F29" s="264"/>
+      <c r="F29" s="273"/>
       <c r="G29" s="72">
         <f>E29/E30</f>
         <v>0.14562655387297796</v>
@@ -6581,17 +6581,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J29" s="264"/>
+      <c r="J29" s="273"/>
       <c r="K29" s="72">
         <f>I29/I30</f>
         <v>0.1276687765161397</v>
       </c>
-      <c r="M29" s="268" t="s">
+      <c r="M29" s="263" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="267"/>
+      <c r="B30" s="268"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
@@ -6600,18 +6600,18 @@
         <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
         <v>154855</v>
       </c>
-      <c r="F30" s="265"/>
+      <c r="F30" s="274"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E32:F32) + AVERAGE(BS!E36:F36) + AVERAGE(BS!E42:F42)</f>
         <v>145666</v>
       </c>
-      <c r="J30" s="265"/>
+      <c r="J30" s="274"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="269"/>
+      <c r="M30" s="264"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="278" t="s">
+      <c r="B33" s="275" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6622,7 +6622,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F33" s="276"/>
+      <c r="F33" s="277"/>
       <c r="G33" s="247">
         <f>E33/E34</f>
         <v>0.14434385449800183</v>
@@ -6632,17 +6632,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J33" s="276"/>
+      <c r="J33" s="277"/>
       <c r="K33" s="247">
         <f>I33/I34</f>
         <v>0.13136687601439562</v>
       </c>
-      <c r="M33" s="268" t="s">
+      <c r="M33" s="263" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="279"/>
+      <c r="B34" s="276"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
@@ -6651,45 +6651,22 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F34" s="277"/>
+      <c r="F34" s="278"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J34" s="277"/>
+      <c r="J34" s="278"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="269"/>
+      <c r="M34" s="264"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6702,6 +6679,29 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6716,7 +6716,7 @@
   <dimension ref="B3:O29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -6727,7 +6727,7 @@
     <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
@@ -6738,22 +6738,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B3" s="270" t="s">
+      <c r="B3" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="270"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="270" t="s">
+      <c r="E3" s="269" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="270" t="s">
+      <c r="I3" s="269" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="272"/>
-      <c r="K3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -6768,7 +6768,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="267" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6779,7 +6779,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F5" s="264"/>
+      <c r="F5" s="273"/>
       <c r="G5" s="71">
         <f>E5/E6</f>
         <v>1.7698000000000003</v>
@@ -6788,17 +6788,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J5" s="264"/>
+      <c r="J5" s="273"/>
       <c r="K5" s="113">
         <f>I5/I6</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="M5" s="268" t="s">
+      <c r="M5" s="263" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="267"/>
+      <c r="B6" s="268"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
@@ -6807,15 +6807,15 @@
         <f>'P&amp;L'!D50</f>
         <v>10000</v>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="274"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>E6</f>
         <v>10000</v>
       </c>
-      <c r="J6" s="265"/>
+      <c r="J6" s="274"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="269"/>
+      <c r="M6" s="264"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6836,7 +6836,7 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="266" t="s">
+      <c r="B9" s="267" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6846,7 +6846,7 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F9" s="264"/>
+      <c r="F9" s="273"/>
       <c r="G9" s="71">
         <f>E9/E10</f>
         <v>1.6668550118657475</v>
@@ -6855,20 +6855,20 @@
         <f>'P&amp;L'!E53</f>
         <v>2.15</v>
       </c>
-      <c r="J9" s="276"/>
+      <c r="J9" s="277"/>
       <c r="K9" s="197">
         <f>I9/I10</f>
         <v>1.5398939979945563</v>
       </c>
       <c r="L9" s="73"/>
-      <c r="M9" s="282" t="s">
+      <c r="M9" s="279" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="267"/>
+      <c r="B10" s="268"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
@@ -6876,16 +6876,16 @@
         <f>G5</f>
         <v>1.7698000000000003</v>
       </c>
-      <c r="F10" s="265"/>
+      <c r="F10" s="274"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198">
         <f>K5</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="J10" s="277"/>
+      <c r="J10" s="278"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="283"/>
+      <c r="M10" s="280"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6899,7 +6899,7 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="266" t="s">
+      <c r="B13" s="267" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6909,7 +6909,7 @@
         <f>'P&amp;L'!D54</f>
         <v>29500</v>
       </c>
-      <c r="F13" s="264"/>
+      <c r="F13" s="273"/>
       <c r="G13" s="71">
         <f>E13/E14</f>
         <v>1.6668550118657472</v>
@@ -6918,17 +6918,17 @@
         <f>'P&amp;L'!E54</f>
         <v>21500</v>
       </c>
-      <c r="J13" s="264"/>
+      <c r="J13" s="273"/>
       <c r="K13" s="113">
         <f>I13/I14</f>
         <v>1.5398939979945563</v>
       </c>
-      <c r="M13" s="268" t="s">
+      <c r="M13" s="263" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="267"/>
+      <c r="B14" s="268"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
@@ -6936,18 +6936,18 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F14" s="265"/>
+      <c r="F14" s="274"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="274"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="269"/>
+      <c r="M14" s="264"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="266" t="s">
+      <c r="B17" s="267" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6957,7 +6957,7 @@
         <f>'P&amp;L'!D51</f>
         <v>0.88</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="250">
         <f>E17/E18</f>
         <v>0.29830508474576267</v>
@@ -6966,17 +6966,17 @@
         <f>'P&amp;L'!E51</f>
         <v>0.65</v>
       </c>
-      <c r="J17" s="264"/>
+      <c r="J17" s="273"/>
       <c r="K17" s="250">
         <f>I17/I18</f>
         <v>0.30232558139534887</v>
       </c>
-      <c r="M17" s="268" t="s">
+      <c r="M17" s="263" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="267"/>
+      <c r="B18" s="268"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
@@ -6984,18 +6984,18 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F18" s="265"/>
+      <c r="F18" s="274"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117">
         <f>I9</f>
         <v>2.15</v>
       </c>
-      <c r="J18" s="265"/>
+      <c r="J18" s="274"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="269"/>
+      <c r="M18" s="264"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="267" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -7005,7 +7005,7 @@
         <f>'P&amp;L'!D32-'P&amp;L'!D52</f>
         <v>8898.0000000000036</v>
       </c>
-      <c r="F21" s="264"/>
+      <c r="F21" s="273"/>
       <c r="G21" s="66">
         <f>E21/E22</f>
         <v>0.50276867442648898</v>
@@ -7014,18 +7014,18 @@
         <f>'P&amp;L'!E32-'P&amp;L'!E52</f>
         <v>7462.0000000000036</v>
       </c>
-      <c r="J21" s="264"/>
+      <c r="J21" s="273"/>
       <c r="K21" s="66">
         <f>I21/I22</f>
         <v>0.53445065176908768</v>
       </c>
-      <c r="M21" s="268" t="s">
+      <c r="M21" s="263" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="267"/>
+      <c r="B22" s="268"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
@@ -7033,18 +7033,18 @@
         <f>E14</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F22" s="265"/>
+      <c r="F22" s="274"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>I14</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J22" s="265"/>
+      <c r="J22" s="274"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="269"/>
+      <c r="M22" s="264"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="266" t="s">
+      <c r="B25" s="267" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -7054,7 +7054,7 @@
         <f>'P&amp;L'!D52</f>
         <v>8800</v>
       </c>
-      <c r="F25" s="264"/>
+      <c r="F25" s="273"/>
       <c r="G25" s="66">
         <f>E25/E26</f>
         <v>0.49723132557351102</v>
@@ -7063,17 +7063,17 @@
         <f>'P&amp;L'!E52</f>
         <v>6500</v>
       </c>
-      <c r="J25" s="264"/>
+      <c r="J25" s="273"/>
       <c r="K25" s="66">
         <f>I25/I26</f>
         <v>0.46554934823091237</v>
       </c>
-      <c r="M25" s="268" t="s">
+      <c r="M25" s="263" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="267"/>
+      <c r="B26" s="268"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
@@ -7081,40 +7081,49 @@
         <f>E22</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F26" s="265"/>
+      <c r="F26" s="274"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J26" s="265"/>
+      <c r="J26" s="274"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="269"/>
+      <c r="M26" s="264"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="280" t="s">
+      <c r="B29" s="281" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="281"/>
+      <c r="C29" s="282"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
-      <c r="G29" s="259"/>
+      <c r="G29" s="300">
+        <f>G21*'Profitability ratios'!G33</f>
+        <v>7.2571568387570382E-2</v>
+      </c>
       <c r="H29" s="138"/>
-      <c r="I29" s="260"/>
+      <c r="I29" s="259"/>
       <c r="J29" s="258"/>
-      <c r="K29" s="259"/>
+      <c r="K29" s="300">
+        <f>K21*'Profitability ratios'!K33</f>
+        <v>7.0209112506762664E-2</v>
+      </c>
       <c r="M29" s="134" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -7128,15 +7137,12 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7168,10 +7174,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="287" t="s">
+      <c r="D2" s="286" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="288"/>
+      <c r="E2" s="287"/>
     </row>
     <row r="3" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="160" t="s">
@@ -7199,7 +7205,7 @@
       <c r="G4" s="163"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="289" t="s">
+      <c r="B5" s="288" t="s">
         <v>256</v>
       </c>
       <c r="C5" s="164" t="s">
@@ -7221,7 +7227,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="290"/>
+      <c r="B6" s="289"/>
       <c r="C6" s="165" t="s">
         <v>253</v>
       </c>
@@ -7242,7 +7248,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="290"/>
+      <c r="B7" s="289"/>
       <c r="C7" s="165" t="s">
         <v>254</v>
       </c>
@@ -7262,7 +7268,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="290"/>
+      <c r="B8" s="289"/>
       <c r="C8" s="165" t="s">
         <v>255</v>
       </c>
@@ -7284,7 +7290,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="291"/>
+      <c r="B9" s="290"/>
       <c r="C9" s="166" t="s">
         <v>88</v>
       </c>
@@ -7308,7 +7314,7 @@
       <c r="G10" s="163"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="284" t="s">
+      <c r="B11" s="283" t="s">
         <v>258</v>
       </c>
       <c r="C11" s="80" t="s">
@@ -7330,7 +7336,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="285"/>
+      <c r="B12" s="284"/>
       <c r="C12" s="35" t="s">
         <v>257</v>
       </c>
@@ -7350,7 +7356,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="286"/>
+      <c r="B13" s="285"/>
       <c r="C13" s="58" t="s">
         <v>266</v>
       </c>
@@ -7374,7 +7380,7 @@
       <c r="G14" s="163"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="284" t="s">
+      <c r="B15" s="283" t="s">
         <v>268</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -7396,7 +7402,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="285"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="35" t="s">
         <v>265</v>
       </c>
@@ -7416,7 +7422,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="286"/>
+      <c r="B17" s="285"/>
       <c r="C17" s="58" t="s">
         <v>267</v>
       </c>
@@ -7441,7 +7447,7 @@
       <c r="G18" s="163"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="284" t="s">
+      <c r="B19" s="283" t="s">
         <v>259</v>
       </c>
       <c r="C19" s="80" t="s">
@@ -7463,7 +7469,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B20" s="285"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="35" t="s">
         <v>269</v>
       </c>
@@ -7483,7 +7489,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="285"/>
+      <c r="B21" s="284"/>
       <c r="C21" s="35" t="s">
         <v>89</v>
       </c>
@@ -7503,7 +7509,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="286"/>
+      <c r="B22" s="285"/>
       <c r="C22" s="58" t="s">
         <v>167</v>
       </c>
@@ -7529,7 +7535,7 @@
       <c r="G23" s="163"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B24" s="284" t="s">
+      <c r="B24" s="283" t="s">
         <v>261</v>
       </c>
       <c r="C24" s="80" t="s">
@@ -7551,7 +7557,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B25" s="285"/>
+      <c r="B25" s="284"/>
       <c r="C25" s="35" t="s">
         <v>263</v>
       </c>
@@ -7571,7 +7577,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B26" s="286"/>
+      <c r="B26" s="285"/>
       <c r="C26" s="58" t="s">
         <v>186</v>
       </c>

</xml_diff>

<commit_message>
Calculating and interpreting Altman's Z score
</commit_message>
<xml_diff>
--- a/salesmart_financial_ratios_model.xlsx
+++ b/salesmart_financial_ratios_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E08BA-63A9-034E-AF7D-AE10FA6A4AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A098AB-8E9D-7643-98A6-3CA161E7CC28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="950" firstSheet="1" activeTab="6" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="950" firstSheet="2" activeTab="11" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -2029,6 +2029,7 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2038,40 +2039,46 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2080,11 +2087,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2092,12 +2099,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2149,7 +2150,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2473,7 +2473,7 @@
   <dimension ref="B3:I49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -2889,17 +2889,17 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="6"/>
-      <c r="C33" s="260"/>
-      <c r="D33" s="261"/>
-      <c r="E33" s="261"/>
+      <c r="C33" s="261"/>
+      <c r="D33" s="262"/>
+      <c r="E33" s="262"/>
     </row>
     <row r="34" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="260"/>
-      <c r="D34" s="262"/>
-      <c r="E34" s="262"/>
+      <c r="C34" s="261"/>
+      <c r="D34" s="263"/>
+      <c r="E34" s="263"/>
     </row>
     <row r="35" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
@@ -3180,13 +3180,13 @@
       <c r="C5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="273" t="s">
+      <c r="D5" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="40" t="s">
@@ -3197,11 +3197,11 @@
       <c r="C6" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="274"/>
+      <c r="D6" s="265"/>
       <c r="E6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="41" t="s">
         <v>94</v>
       </c>
@@ -3286,19 +3286,19 @@
       <c r="C14" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="273" t="s">
+      <c r="D14" s="264" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="273" t="s">
+      <c r="F14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="273" t="s">
+      <c r="H14" s="264" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3311,15 +3311,15 @@
       <c r="C15" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="274"/>
+      <c r="D15" s="265"/>
       <c r="E15" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="274"/>
+      <c r="F15" s="265"/>
       <c r="G15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="274"/>
+      <c r="H15" s="265"/>
       <c r="I15" s="85" t="s">
         <v>94</v>
       </c>
@@ -3428,31 +3428,31 @@
       <c r="C23" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="291" t="s">
+      <c r="D23" s="292" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="291" t="s">
+      <c r="F23" s="292" t="s">
         <v>97</v>
       </c>
       <c r="G23" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="291" t="s">
+      <c r="H23" s="292" t="s">
         <v>97</v>
       </c>
       <c r="I23" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="291" t="s">
+      <c r="J23" s="292" t="s">
         <v>97</v>
       </c>
       <c r="K23" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="291" t="s">
+      <c r="L23" s="292" t="s">
         <v>97</v>
       </c>
       <c r="M23" s="90" t="s">
@@ -3463,23 +3463,23 @@
       <c r="C24" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="292"/>
+      <c r="D24" s="293"/>
       <c r="E24" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="292"/>
+      <c r="F24" s="293"/>
       <c r="G24" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="292"/>
+      <c r="H24" s="293"/>
       <c r="I24" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="292"/>
+      <c r="J24" s="293"/>
       <c r="K24" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="292"/>
+      <c r="L24" s="293"/>
       <c r="M24" s="93" t="s">
         <v>94</v>
       </c>
@@ -3559,16 +3559,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3582,8 +3582,8 @@
   </sheetPr>
   <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3599,14 +3599,14 @@
   <sheetData>
     <row r="2" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="293" t="s">
+      <c r="D3" s="294" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="294"/>
-      <c r="F3" s="295" t="s">
+      <c r="E3" s="295"/>
+      <c r="F3" s="296" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="296"/>
+      <c r="G3" s="297"/>
     </row>
     <row r="4" spans="2:14" s="142" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="251" t="s">
@@ -3638,10 +3638,22 @@
       <c r="C5" s="235">
         <v>1.2</v>
       </c>
-      <c r="D5" s="237"/>
-      <c r="E5" s="238"/>
-      <c r="F5" s="237"/>
-      <c r="G5" s="238"/>
+      <c r="D5" s="237">
+        <f>(BS!D22-BS!D45)/BS!D23</f>
+        <v>0.21741769246472928</v>
+      </c>
+      <c r="E5" s="238">
+        <f>C5*D5</f>
+        <v>0.26090123095767515</v>
+      </c>
+      <c r="F5" s="237">
+        <f>(BS!E22-BS!E45)/BS!E23</f>
+        <v>0.17068401973019551</v>
+      </c>
+      <c r="G5" s="238">
+        <f>C5*F5</f>
+        <v>0.20482082367623461</v>
+      </c>
       <c r="H5" s="232" t="s">
         <v>215</v>
       </c>
@@ -3653,10 +3665,22 @@
       <c r="C6" s="204">
         <v>1.4</v>
       </c>
-      <c r="D6" s="226"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="205"/>
+      <c r="D6" s="226">
+        <f>BS!D29/BS!D23</f>
+        <v>0.33734640616637518</v>
+      </c>
+      <c r="E6" s="205">
+        <f t="shared" ref="E6:E9" si="0">C6*D6</f>
+        <v>0.47228496863292524</v>
+      </c>
+      <c r="F6" s="226">
+        <f>BS!E29/BS!E23</f>
+        <v>0.30013668508943958</v>
+      </c>
+      <c r="G6" s="205">
+        <f t="shared" ref="G6:G9" si="1">C6*F6</f>
+        <v>0.42019135912521538</v>
+      </c>
       <c r="H6" s="206" t="s">
         <v>216</v>
       </c>
@@ -3668,10 +3692,22 @@
       <c r="C7" s="204">
         <v>3.3</v>
       </c>
-      <c r="D7" s="226"/>
-      <c r="E7" s="205"/>
-      <c r="F7" s="226"/>
-      <c r="G7" s="205"/>
+      <c r="D7" s="226">
+        <f>'P&amp;L'!D24/BS!D23</f>
+        <v>0.12442548871392237</v>
+      </c>
+      <c r="E7" s="205">
+        <f t="shared" si="0"/>
+        <v>0.41060411275594377</v>
+      </c>
+      <c r="F7" s="226">
+        <f>'P&amp;L'!E24/BS!E23</f>
+        <v>0.1105188090568729</v>
+      </c>
+      <c r="G7" s="205">
+        <f t="shared" si="1"/>
+        <v>0.36471206988768057</v>
+      </c>
       <c r="H7" s="206" t="s">
         <v>217</v>
       </c>
@@ -3683,10 +3719,22 @@
       <c r="C8" s="239">
         <v>1</v>
       </c>
-      <c r="D8" s="226"/>
-      <c r="E8" s="205"/>
-      <c r="F8" s="226"/>
-      <c r="G8" s="205"/>
+      <c r="D8" s="226">
+        <f>'P&amp;L'!D13/BS!D23</f>
+        <v>1.0971303402651718</v>
+      </c>
+      <c r="E8" s="205">
+        <f t="shared" si="0"/>
+        <v>1.0971303402651718</v>
+      </c>
+      <c r="F8" s="226">
+        <f>'P&amp;L'!E13/BS!E23</f>
+        <v>1.0705473346407559</v>
+      </c>
+      <c r="G8" s="205">
+        <f t="shared" si="1"/>
+        <v>1.0705473346407559</v>
+      </c>
       <c r="H8" s="206" t="s">
         <v>220</v>
       </c>
@@ -3698,10 +3746,22 @@
       <c r="C9" s="236">
         <v>0.6</v>
       </c>
-      <c r="D9" s="227"/>
-      <c r="E9" s="208"/>
-      <c r="F9" s="227"/>
-      <c r="G9" s="208"/>
+      <c r="D9" s="227">
+        <f>'P&amp;L'!D54/BS!D46</f>
+        <v>0.59233379515290241</v>
+      </c>
+      <c r="E9" s="208">
+        <f t="shared" si="0"/>
+        <v>0.35540027709174143</v>
+      </c>
+      <c r="F9" s="227">
+        <f>'P&amp;L'!E54/BS!E46</f>
+        <v>0.39458229334899425</v>
+      </c>
+      <c r="G9" s="208">
+        <f t="shared" si="1"/>
+        <v>0.23674937600939655</v>
+      </c>
       <c r="H9" s="209" t="s">
         <v>218</v>
       </c>
@@ -3712,9 +3772,15 @@
       </c>
       <c r="C10" s="229"/>
       <c r="D10" s="207"/>
-      <c r="E10" s="230"/>
+      <c r="E10" s="230">
+        <f>SUM(E5:E9)</f>
+        <v>2.5963209297034573</v>
+      </c>
       <c r="F10" s="210"/>
-      <c r="G10" s="230"/>
+      <c r="G10" s="230">
+        <f>SUM(G5:G9)</f>
+        <v>2.2970209633392829</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.15">
       <c r="N11" s="3" t="s">
@@ -3738,7 +3804,7 @@
   </sheetPr>
   <dimension ref="B3:S18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3754,16 +3820,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="C3" s="297" t="s">
+      <c r="C3" s="298" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="298"/>
-      <c r="E3" s="298"/>
-      <c r="F3" s="297" t="s">
+      <c r="D3" s="299"/>
+      <c r="E3" s="299"/>
+      <c r="F3" s="298" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="298"/>
-      <c r="H3" s="299"/>
+      <c r="G3" s="299"/>
+      <c r="H3" s="300"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B4" s="142"/>
@@ -3976,16 +4042,16 @@
       <c r="G11" s="139"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="C13" s="297" t="s">
+      <c r="C13" s="298" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="298"/>
-      <c r="E13" s="299"/>
-      <c r="F13" s="297" t="s">
+      <c r="D13" s="299"/>
+      <c r="E13" s="300"/>
+      <c r="F13" s="298" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="298"/>
-      <c r="H13" s="299"/>
+      <c r="G13" s="299"/>
+      <c r="H13" s="300"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C14" s="255" t="s">
@@ -4135,7 +4201,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E57" sqref="E57"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4730,22 +4796,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="270" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="270"/>
+      <c r="C3" s="271"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="270" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="271"/>
-      <c r="G3" s="270"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="269" t="s">
+      <c r="I3" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="271"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -4753,7 +4819,7 @@
       <c r="O3" s="156"/>
     </row>
     <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="266" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4763,7 +4829,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F5" s="273"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>7.8186929852154767</v>
@@ -4772,17 +4838,17 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J5" s="273"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="268" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="268"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>42</v>
       </c>
@@ -4790,15 +4856,15 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
@@ -4809,7 +4875,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="267" t="s">
+      <c r="B9" s="266" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="40">
@@ -4819,7 +4885,7 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="F9" s="273"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>46.682994292036511</v>
@@ -4828,17 +4894,17 @@
         <f>C9</f>
         <v>365</v>
       </c>
-      <c r="J9" s="273"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>51.396350636445895</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="268" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="268"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>44</v>
       </c>
@@ -4846,15 +4912,15 @@
         <f>G5</f>
         <v>7.8186929852154767</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="264"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
@@ -4865,7 +4931,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="266" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4875,7 +4941,7 @@
         <f>'P&amp;L'!D15 * -1</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="273"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="44">
         <f>E13/E14</f>
         <v>6.1185026563804019</v>
@@ -4884,17 +4950,17 @@
         <f>'P&amp;L'!E15 * -1</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="273"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="268" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="268"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>46</v>
       </c>
@@ -4902,15 +4968,15 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
@@ -4921,7 +4987,7 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="266" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="40">
@@ -4931,7 +4997,7 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>59.655118335100561</v>
@@ -4940,17 +5006,17 @@
         <f>C17</f>
         <v>365</v>
       </c>
-      <c r="J17" s="273"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="268" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="268"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>48</v>
       </c>
@@ -4958,15 +5024,15 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
@@ -4977,7 +5043,7 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="266" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4987,7 +5053,7 @@
         <f>BS!D18-BS!E18-'P&amp;L'!D15</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="273"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="44">
         <f>E21/E22</f>
         <v>8.2567109661638813</v>
@@ -4996,12 +5062,12 @@
         <f>BS!E18-BS!F18-'P&amp;L'!E15</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="273"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="268" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -5009,7 +5075,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="268"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>51</v>
       </c>
@@ -5017,15 +5083,15 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
@@ -5036,7 +5102,7 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B25" s="267" t="s">
+      <c r="B25" s="266" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="40">
@@ -5046,7 +5112,7 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="F25" s="273"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="53">
         <f>E25/E26</f>
         <v>44.20646447426526</v>
@@ -5055,17 +5121,17 @@
         <f>C25</f>
         <v>365</v>
       </c>
-      <c r="J25" s="273"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="265" t="s">
+      <c r="M25" s="274" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B26" s="268"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>52</v>
       </c>
@@ -5073,15 +5139,15 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="266"/>
+      <c r="M26" s="275"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
@@ -5092,7 +5158,7 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="266" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -5102,7 +5168,7 @@
         <f>E5</f>
         <v>198845</v>
       </c>
-      <c r="F29" s="273"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="44">
         <f>E29/E30</f>
         <v>1.8745787159025025</v>
@@ -5111,17 +5177,17 @@
         <f>I5</f>
         <v>180141</v>
       </c>
-      <c r="J29" s="273"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="44">
         <f>I29/I30</f>
         <v>1.72279045747321</v>
       </c>
-      <c r="M29" s="263" t="s">
+      <c r="M29" s="268" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B30" s="268"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>55</v>
       </c>
@@ -5129,15 +5195,15 @@
         <f>AVERAGE(BS!D11:E11)</f>
         <v>106074.5</v>
       </c>
-      <c r="F30" s="274"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E11:F11)</f>
         <v>104563.5</v>
       </c>
-      <c r="J30" s="274"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="264"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
@@ -5148,7 +5214,7 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B33" s="267" t="s">
+      <c r="B33" s="266" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="40" t="s">
@@ -5158,7 +5224,7 @@
         <f>E29</f>
         <v>198845</v>
       </c>
-      <c r="F33" s="273"/>
+      <c r="F33" s="264"/>
       <c r="G33" s="44">
         <f>E33/E34</f>
         <v>5.8375656871091799</v>
@@ -5167,17 +5233,17 @@
         <f>I29</f>
         <v>180141</v>
       </c>
-      <c r="J33" s="273"/>
+      <c r="J33" s="264"/>
       <c r="K33" s="44">
         <f>I33/I34</f>
         <v>7.4487677803506447</v>
       </c>
-      <c r="M33" s="263" t="s">
+      <c r="M33" s="268" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="268"/>
+      <c r="B34" s="267"/>
       <c r="C34" s="41" t="s">
         <v>56</v>
       </c>
@@ -5185,15 +5251,15 @@
         <f>AVERAGE(BS!D22:E22) - AVERAGE(BS!D45:E45)</f>
         <v>34063</v>
       </c>
-      <c r="F34" s="274"/>
+      <c r="F34" s="265"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45">
         <f>AVERAGE(BS!E22:F22)-AVERAGE(BS!E45:F45)</f>
         <v>24184</v>
       </c>
-      <c r="J34" s="274"/>
+      <c r="J34" s="265"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="264"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
@@ -5210,7 +5276,7 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="267" t="s">
+      <c r="B37" s="266" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="40" t="s">
@@ -5220,7 +5286,7 @@
         <f>E33</f>
         <v>198845</v>
       </c>
-      <c r="F37" s="273"/>
+      <c r="F37" s="264"/>
       <c r="G37" s="44">
         <f>E37/E38</f>
         <v>1.1378468774945567</v>
@@ -5229,17 +5295,17 @@
         <f>I33</f>
         <v>180141</v>
       </c>
-      <c r="J37" s="273"/>
+      <c r="J37" s="264"/>
       <c r="K37" s="44">
         <f>I37/I38</f>
         <v>1.0923495329312995</v>
       </c>
-      <c r="M37" s="263" t="s">
+      <c r="M37" s="268" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B38" s="268"/>
+      <c r="B38" s="267"/>
       <c r="C38" s="41" t="s">
         <v>54</v>
       </c>
@@ -5247,15 +5313,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F38" s="274"/>
+      <c r="F38" s="265"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J38" s="274"/>
+      <c r="J38" s="265"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="264"/>
+      <c r="M38" s="269"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
@@ -5291,7 +5357,7 @@
         <f>I41+I43-I45</f>
         <v>66.374159453238519</v>
       </c>
-      <c r="M41" s="263" t="s">
+      <c r="M41" s="268" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5305,7 +5371,7 @@
       <c r="I42" s="54"/>
       <c r="J42" s="35"/>
       <c r="K42" s="50"/>
-      <c r="M42" s="272"/>
+      <c r="M42" s="273"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B43" s="49"/>
@@ -5325,7 +5391,7 @@
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="50"/>
-      <c r="M43" s="272"/>
+      <c r="M43" s="273"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B44" s="49"/>
@@ -5336,7 +5402,7 @@
       <c r="I44" s="54"/>
       <c r="J44" s="56"/>
       <c r="K44" s="50"/>
-      <c r="M44" s="272"/>
+      <c r="M44" s="273"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B45" s="51"/>
@@ -5355,14 +5421,14 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="264"/>
+      <c r="M45" s="269"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="267" t="s">
+      <c r="B48" s="266" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="40" t="s">
@@ -5372,7 +5438,7 @@
         <f>E37</f>
         <v>198845</v>
       </c>
-      <c r="F48" s="273"/>
+      <c r="F48" s="264"/>
       <c r="G48" s="44">
         <f>E48/E49</f>
         <v>1.6217682081396296</v>
@@ -5381,17 +5447,17 @@
         <f>I37</f>
         <v>180141</v>
       </c>
-      <c r="J48" s="273"/>
+      <c r="J48" s="264"/>
       <c r="K48" s="44">
         <f>I48/I49</f>
         <v>1.6949262578505397</v>
       </c>
-      <c r="M48" s="263" t="s">
+      <c r="M48" s="268" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B49" s="268"/>
+      <c r="B49" s="267"/>
       <c r="C49" s="41" t="s">
         <v>74</v>
       </c>
@@ -5399,18 +5465,46 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F49" s="274"/>
+      <c r="F49" s="265"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J49" s="274"/>
+      <c r="J49" s="265"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="264"/>
+      <c r="M49" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F37:F38"/>
@@ -5427,34 +5521,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5491,29 +5557,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="270" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="270"/>
+      <c r="C3" s="271"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="270" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="271"/>
-      <c r="G3" s="270"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="269" t="s">
+      <c r="I3" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="271"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="266" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5524,7 +5590,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="273"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="53">
         <f>E5/E6</f>
         <v>2.250872960446956</v>
@@ -5533,17 +5599,17 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="273"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="265" t="s">
+      <c r="M5" s="274" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="268"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
@@ -5552,18 +5618,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="266"/>
+      <c r="M6" s="275"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="267" t="s">
+      <c r="B9" s="266" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5574,7 +5640,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="273"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="53">
         <f>E9/E10</f>
         <v>1.4455590121262143</v>
@@ -5583,17 +5649,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="273"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="265" t="s">
+      <c r="M9" s="274" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="268"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>59</v>
       </c>
@@ -5602,18 +5668,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="266"/>
+      <c r="M10" s="275"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="266" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5624,7 +5690,7 @@
         <f>SUM((BS!D20:D21))</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="273"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="53">
         <f>E13/E14</f>
         <v>0.61237381753539455</v>
@@ -5633,17 +5699,17 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="273"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="53">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="265" t="s">
+      <c r="M13" s="274" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="268"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
@@ -5652,18 +5718,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="266"/>
+      <c r="M14" s="275"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="266" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5674,7 +5740,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="53">
         <f>E17/E18</f>
         <v>94.282108296368563</v>
@@ -5683,17 +5749,17 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="273"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="265" t="s">
+      <c r="M17" s="274" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="268"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>65</v>
       </c>
@@ -5702,27 +5768,18 @@
         <f>('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/-365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/-365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="266"/>
+      <c r="M18" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5733,6 +5790,15 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5769,29 +5835,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="270" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="270"/>
+      <c r="C3" s="271"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="270" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="271"/>
-      <c r="G3" s="270"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="269" t="s">
+      <c r="I3" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="271"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="266" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5802,7 +5868,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="273"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="66">
         <f>E5/E6</f>
         <v>0.2242426086824206</v>
@@ -5811,17 +5877,17 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="273"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="268" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="268"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>70</v>
       </c>
@@ -5830,15 +5896,15 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="264"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -5857,7 +5923,7 @@
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="267" t="s">
+      <c r="B9" s="266" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5868,7 +5934,7 @@
         <f>E5</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="273"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="66">
         <f>E9/E10</f>
         <v>0.18316843989261211</v>
@@ -5877,17 +5943,17 @@
         <f>I5</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="273"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="268" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="268"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
@@ -5896,15 +5962,15 @@
         <f>BS!D32+BS!D36+BS!D42</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>I6+I5</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="264"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
@@ -5913,7 +5979,7 @@
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="266" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5924,7 +5990,7 @@
         <f>E9</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="273"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="66">
         <f>E13/E14</f>
         <v>0.16262324749918616</v>
@@ -5933,17 +5999,17 @@
         <f>I9</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="273"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="268" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="268"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>72</v>
       </c>
@@ -5952,15 +6018,15 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="264"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
@@ -5969,7 +6035,7 @@
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="266" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5980,7 +6046,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="71">
         <f>E17/E18</f>
         <v>8.2755963302752313</v>
@@ -5989,17 +6055,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="273"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="268" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="268"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>76</v>
       </c>
@@ -6008,15 +6074,15 @@
         <f>'P&amp;L'!D26 * -1</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>'P&amp;L'!E26*-1</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="264"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
@@ -6025,7 +6091,7 @@
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="266" t="s">
         <v>279</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6036,7 +6102,7 @@
         <f>'P&amp;L'!D24+'P&amp;L'!D55*-1</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="273"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="71">
         <f>E21/E22</f>
         <v>4.9604474630443471</v>
@@ -6045,17 +6111,17 @@
         <f>'P&amp;L'!E24+'P&amp;L'!E55*-1</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="273"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="268" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="268"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
@@ -6064,21 +6130,21 @@
         <f>'P&amp;L'!D26*-1 +'P&amp;L'!D55*-1</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-1*('P&amp;L'!E55+'P&amp;L'!E26)</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="264"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="267" t="s">
+      <c r="B25" s="266" t="s">
         <v>280</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6089,7 +6155,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="273"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="71">
         <f>E25/E26</f>
         <v>1.4252956528831253</v>
@@ -6098,17 +6164,17 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="273"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="268" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="268"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>74</v>
       </c>
@@ -6117,28 +6183,25 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="264"/>
+      <c r="M26" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -6149,13 +6212,16 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6192,22 +6258,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="270" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="270"/>
+      <c r="C3" s="271"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="270" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="271"/>
-      <c r="G3" s="270"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="269" t="s">
+      <c r="I3" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="271"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -6221,7 +6287,7 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="266" t="s">
         <v>173</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6232,7 +6298,7 @@
         <f>'P&amp;L'!D17</f>
         <v>48553.16</v>
       </c>
-      <c r="F5" s="273"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="72">
         <f>E5/E6</f>
         <v>0.24417591591440571</v>
@@ -6241,17 +6307,17 @@
         <f>'P&amp;L'!E17</f>
         <v>41525.160000000003</v>
       </c>
-      <c r="J5" s="273"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="72">
         <f>I5/I6</f>
         <v>0.23051476343530902</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="268" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B6" s="268"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>53</v>
       </c>
@@ -6260,15 +6326,15 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
@@ -6285,7 +6351,7 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="267" t="s">
+      <c r="B9" s="266" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6296,7 +6362,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F9" s="273"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="72">
         <f>E9/E10</f>
         <v>0.11340994241746086</v>
@@ -6305,17 +6371,17 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J9" s="273"/>
+      <c r="J9" s="264"/>
       <c r="K9" s="72">
         <f>I9/I10</f>
         <v>0.1032357986244109</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="268" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="268"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>53</v>
       </c>
@@ -6324,15 +6390,15 @@
         <f>E6</f>
         <v>198845</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>I6</f>
         <v>180141</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="265"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="264"/>
+      <c r="M10" s="269"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
@@ -6349,7 +6415,7 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="266" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6360,7 +6426,7 @@
         <f>'P&amp;L'!D28</f>
         <v>19826.000000000004</v>
       </c>
-      <c r="F13" s="273"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="72">
         <f>E13/E14</f>
         <v>9.9705801000779526E-2</v>
@@ -6369,17 +6435,17 @@
         <f>'P&amp;L'!E28</f>
         <v>15605.000000000004</v>
       </c>
-      <c r="J13" s="273"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="72">
         <f>I13/I14</f>
         <v>8.6626586951332588E-2</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="268" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B14" s="268"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>53</v>
       </c>
@@ -6388,18 +6454,18 @@
         <f>E10</f>
         <v>198845</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>I10</f>
         <v>180141</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="266" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6410,7 +6476,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="72">
         <f>E17/E18</f>
         <v>8.9003998088963782E-2</v>
@@ -6419,17 +6485,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J17" s="273"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="72">
         <f>I17/I18</f>
         <v>7.7505953669625482E-2</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="268" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="268"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>53</v>
       </c>
@@ -6438,18 +6504,18 @@
         <f>E14</f>
         <v>198845</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>I14</f>
         <v>180141</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="266" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6460,7 +6526,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F21" s="273"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="72">
         <f>E21/E22</f>
         <v>0.10127292131005892</v>
@@ -6469,17 +6535,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J21" s="273"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="72">
         <f>I21/I22</f>
         <v>8.4663592290410331E-2</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="268" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B22" s="268"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>54</v>
       </c>
@@ -6488,15 +6554,15 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
@@ -6511,7 +6577,7 @@
       <c r="M23" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="267" t="s">
+      <c r="B25" s="266" t="s">
         <v>148</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6522,7 +6588,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F25" s="273"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="72">
         <f>E25/E26</f>
         <v>0.1290431488565453</v>
@@ -6531,17 +6597,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J25" s="273"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="72">
         <f>I25/I26</f>
         <v>0.11276957640916493</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="268" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="268"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>54</v>
       </c>
@@ -6550,18 +6616,18 @@
         <f>E22</f>
         <v>174755.5</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>164911.5</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="264"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="266" t="s">
         <v>156</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6572,7 +6638,7 @@
         <f>E9</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F29" s="273"/>
+      <c r="F29" s="264"/>
       <c r="G29" s="72">
         <f>E29/E30</f>
         <v>0.14562655387297796</v>
@@ -6581,17 +6647,17 @@
         <f>I9</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J29" s="273"/>
+      <c r="J29" s="264"/>
       <c r="K29" s="72">
         <f>I29/I30</f>
         <v>0.1276687765161397</v>
       </c>
-      <c r="M29" s="263" t="s">
+      <c r="M29" s="268" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B30" s="268"/>
+      <c r="B30" s="267"/>
       <c r="C30" s="41" t="s">
         <v>84</v>
       </c>
@@ -6600,18 +6666,18 @@
         <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
         <v>154855</v>
       </c>
-      <c r="F30" s="274"/>
+      <c r="F30" s="265"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E32:F32) + AVERAGE(BS!E36:F36) + AVERAGE(BS!E42:F42)</f>
         <v>145666</v>
       </c>
-      <c r="J30" s="274"/>
+      <c r="J30" s="265"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="264"/>
+      <c r="M30" s="269"/>
     </row>
     <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="275" t="s">
+      <c r="B33" s="278" t="s">
         <v>166</v>
       </c>
       <c r="C33" s="245" t="s">
@@ -6622,7 +6688,7 @@
         <f>E17</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F33" s="277"/>
+      <c r="F33" s="276"/>
       <c r="G33" s="247">
         <f>E33/E34</f>
         <v>0.14434385449800183</v>
@@ -6632,17 +6698,17 @@
         <f>I17</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J33" s="277"/>
+      <c r="J33" s="276"/>
       <c r="K33" s="247">
         <f>I33/I34</f>
         <v>0.13136687601439562</v>
       </c>
-      <c r="M33" s="263" t="s">
+      <c r="M33" s="268" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B34" s="276"/>
+      <c r="B34" s="279"/>
       <c r="C34" s="248" t="s">
         <v>94</v>
       </c>
@@ -6651,22 +6717,45 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F34" s="278"/>
+      <c r="F34" s="277"/>
       <c r="G34" s="199"/>
       <c r="H34" s="73"/>
       <c r="I34" s="249">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J34" s="278"/>
+      <c r="J34" s="277"/>
       <c r="K34" s="199"/>
-      <c r="M34" s="264"/>
+      <c r="M34" s="269"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6679,29 +6768,6 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6715,7 +6781,7 @@
   </sheetPr>
   <dimension ref="B3:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -6738,22 +6804,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="270" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="270"/>
+      <c r="C3" s="271"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="269" t="s">
+      <c r="E3" s="270" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="271"/>
-      <c r="G3" s="270"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="269" t="s">
+      <c r="I3" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="271"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271"/>
       <c r="L3" s="68"/>
       <c r="M3" s="69" t="s">
         <v>115</v>
@@ -6768,7 +6834,7 @@
       <c r="M4" s="76"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="267" t="s">
+      <c r="B5" s="266" t="s">
         <v>179</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6779,7 +6845,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F5" s="273"/>
+      <c r="F5" s="264"/>
       <c r="G5" s="71">
         <f>E5/E6</f>
         <v>1.7698000000000003</v>
@@ -6788,17 +6854,17 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J5" s="273"/>
+      <c r="J5" s="264"/>
       <c r="K5" s="113">
         <f>I5/I6</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="268" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B6" s="268"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="41" t="s">
         <v>181</v>
       </c>
@@ -6807,15 +6873,15 @@
         <f>'P&amp;L'!D50</f>
         <v>10000</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="265"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>E6</f>
         <v>10000</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="265"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
@@ -6836,7 +6902,7 @@
       <c r="O8" s="73"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B9" s="267" t="s">
+      <c r="B9" s="266" t="s">
         <v>185</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6846,7 +6912,7 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F9" s="273"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="71">
         <f>E9/E10</f>
         <v>1.6668550118657475</v>
@@ -6855,20 +6921,20 @@
         <f>'P&amp;L'!E53</f>
         <v>2.15</v>
       </c>
-      <c r="J9" s="277"/>
+      <c r="J9" s="276"/>
       <c r="K9" s="197">
         <f>I9/I10</f>
         <v>1.5398939979945563</v>
       </c>
       <c r="L9" s="73"/>
-      <c r="M9" s="279" t="s">
+      <c r="M9" s="282" t="s">
         <v>189</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B10" s="268"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="41" t="s">
         <v>187</v>
       </c>
@@ -6876,16 +6942,16 @@
         <f>G5</f>
         <v>1.7698000000000003</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="46"/>
       <c r="I10" s="198">
         <f>K5</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="J10" s="278"/>
+      <c r="J10" s="277"/>
       <c r="K10" s="199"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="280"/>
+      <c r="M10" s="283"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
@@ -6899,7 +6965,7 @@
       <c r="O11" s="73"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="266" t="s">
         <v>192</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6909,7 +6975,7 @@
         <f>'P&amp;L'!D54</f>
         <v>29500</v>
       </c>
-      <c r="F13" s="273"/>
+      <c r="F13" s="264"/>
       <c r="G13" s="71">
         <f>E13/E14</f>
         <v>1.6668550118657472</v>
@@ -6918,17 +6984,17 @@
         <f>'P&amp;L'!E54</f>
         <v>21500</v>
       </c>
-      <c r="J13" s="273"/>
+      <c r="J13" s="264"/>
       <c r="K13" s="113">
         <f>I13/I14</f>
         <v>1.5398939979945563</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="268" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="268"/>
+      <c r="B14" s="267"/>
       <c r="C14" s="41" t="s">
         <v>95</v>
       </c>
@@ -6936,18 +7002,18 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="265"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="265"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
+      <c r="M14" s="269"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="266" t="s">
         <v>193</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6957,7 +7023,7 @@
         <f>'P&amp;L'!D51</f>
         <v>0.88</v>
       </c>
-      <c r="F17" s="273"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="250">
         <f>E17/E18</f>
         <v>0.29830508474576267</v>
@@ -6966,17 +7032,17 @@
         <f>'P&amp;L'!E51</f>
         <v>0.65</v>
       </c>
-      <c r="J17" s="273"/>
+      <c r="J17" s="264"/>
       <c r="K17" s="250">
         <f>I17/I18</f>
         <v>0.30232558139534887</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="268" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="268"/>
+      <c r="B18" s="267"/>
       <c r="C18" s="41" t="s">
         <v>194</v>
       </c>
@@ -6984,18 +7050,18 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="265"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117">
         <f>I9</f>
         <v>2.15</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="265"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
+      <c r="M18" s="269"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="266" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -7005,7 +7071,7 @@
         <f>'P&amp;L'!D32-'P&amp;L'!D52</f>
         <v>8898.0000000000036</v>
       </c>
-      <c r="F21" s="273"/>
+      <c r="F21" s="264"/>
       <c r="G21" s="66">
         <f>E21/E22</f>
         <v>0.50276867442648898</v>
@@ -7014,18 +7080,18 @@
         <f>'P&amp;L'!E32-'P&amp;L'!E52</f>
         <v>7462.0000000000036</v>
       </c>
-      <c r="J21" s="273"/>
+      <c r="J21" s="264"/>
       <c r="K21" s="66">
         <f>I21/I22</f>
         <v>0.53445065176908768</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="268" t="s">
         <v>202</v>
       </c>
       <c r="O21" s="130"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="268"/>
+      <c r="B22" s="267"/>
       <c r="C22" s="41" t="s">
         <v>200</v>
       </c>
@@ -7033,18 +7099,18 @@
         <f>E14</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="265"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>I14</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="265"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
+      <c r="M22" s="269"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="267" t="s">
+      <c r="B25" s="266" t="s">
         <v>203</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -7054,7 +7120,7 @@
         <f>'P&amp;L'!D52</f>
         <v>8800</v>
       </c>
-      <c r="F25" s="273"/>
+      <c r="F25" s="264"/>
       <c r="G25" s="66">
         <f>E25/E26</f>
         <v>0.49723132557351102</v>
@@ -7063,17 +7129,17 @@
         <f>'P&amp;L'!E52</f>
         <v>6500</v>
       </c>
-      <c r="J25" s="273"/>
+      <c r="J25" s="264"/>
       <c r="K25" s="66">
         <f>I25/I26</f>
         <v>0.46554934823091237</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="268" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B26" s="268"/>
+      <c r="B26" s="267"/>
       <c r="C26" s="41" t="s">
         <v>200</v>
       </c>
@@ -7081,31 +7147,31 @@
         <f>E22</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="265"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="265"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="264"/>
+      <c r="M26" s="269"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B29" s="281" t="s">
+      <c r="B29" s="280" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="282"/>
+      <c r="C29" s="281"/>
       <c r="E29" s="133"/>
       <c r="F29" s="258"/>
-      <c r="G29" s="300">
+      <c r="G29" s="260">
         <f>G21*'Profitability ratios'!G33</f>
         <v>7.2571568387570382E-2</v>
       </c>
       <c r="H29" s="138"/>
       <c r="I29" s="259"/>
       <c r="J29" s="258"/>
-      <c r="K29" s="300">
+      <c r="K29" s="260">
         <f>K21*'Profitability ratios'!K33</f>
         <v>7.0209112506762664E-2</v>
       </c>
@@ -7115,15 +7181,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -7137,12 +7200,15 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7174,10 +7240,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="286" t="s">
+      <c r="D2" s="287" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="287"/>
+      <c r="E2" s="288"/>
     </row>
     <row r="3" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="160" t="s">
@@ -7205,7 +7271,7 @@
       <c r="G4" s="163"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="288" t="s">
+      <c r="B5" s="289" t="s">
         <v>256</v>
       </c>
       <c r="C5" s="164" t="s">
@@ -7227,7 +7293,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="289"/>
+      <c r="B6" s="290"/>
       <c r="C6" s="165" t="s">
         <v>253</v>
       </c>
@@ -7248,7 +7314,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="289"/>
+      <c r="B7" s="290"/>
       <c r="C7" s="165" t="s">
         <v>254</v>
       </c>
@@ -7268,7 +7334,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="289"/>
+      <c r="B8" s="290"/>
       <c r="C8" s="165" t="s">
         <v>255</v>
       </c>
@@ -7290,7 +7356,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="290"/>
+      <c r="B9" s="291"/>
       <c r="C9" s="166" t="s">
         <v>88</v>
       </c>
@@ -7314,7 +7380,7 @@
       <c r="G10" s="163"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="283" t="s">
+      <c r="B11" s="284" t="s">
         <v>258</v>
       </c>
       <c r="C11" s="80" t="s">
@@ -7336,7 +7402,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="284"/>
+      <c r="B12" s="285"/>
       <c r="C12" s="35" t="s">
         <v>257</v>
       </c>
@@ -7356,7 +7422,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="285"/>
+      <c r="B13" s="286"/>
       <c r="C13" s="58" t="s">
         <v>266</v>
       </c>
@@ -7380,7 +7446,7 @@
       <c r="G14" s="163"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="283" t="s">
+      <c r="B15" s="284" t="s">
         <v>268</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -7402,7 +7468,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="284"/>
+      <c r="B16" s="285"/>
       <c r="C16" s="35" t="s">
         <v>265</v>
       </c>
@@ -7422,7 +7488,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="285"/>
+      <c r="B17" s="286"/>
       <c r="C17" s="58" t="s">
         <v>267</v>
       </c>
@@ -7447,7 +7513,7 @@
       <c r="G18" s="163"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="283" t="s">
+      <c r="B19" s="284" t="s">
         <v>259</v>
       </c>
       <c r="C19" s="80" t="s">
@@ -7469,7 +7535,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B20" s="284"/>
+      <c r="B20" s="285"/>
       <c r="C20" s="35" t="s">
         <v>269</v>
       </c>
@@ -7489,7 +7555,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="284"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="35" t="s">
         <v>89</v>
       </c>
@@ -7509,7 +7575,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="285"/>
+      <c r="B22" s="286"/>
       <c r="C22" s="58" t="s">
         <v>167</v>
       </c>
@@ -7535,7 +7601,7 @@
       <c r="G23" s="163"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B24" s="283" t="s">
+      <c r="B24" s="284" t="s">
         <v>261</v>
       </c>
       <c r="C24" s="80" t="s">
@@ -7557,7 +7623,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B25" s="284"/>
+      <c r="B25" s="285"/>
       <c r="C25" s="35" t="s">
         <v>263</v>
       </c>
@@ -7577,7 +7643,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B26" s="285"/>
+      <c r="B26" s="286"/>
       <c r="C26" s="58" t="s">
         <v>186</v>
       </c>

</xml_diff>